<commit_message>
work from current directory
</commit_message>
<xml_diff>
--- a/app/placed_bets.xlsx
+++ b/app/placed_bets.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -140,6 +140,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -507,7 +510,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,7 +520,7 @@
   <cols>
     <col width="17" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
@@ -681,31 +684,83 @@
         <v>1</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="O2" s="2" t="n">
         <v>100</v>
-      </c>
-      <c r="O2" s="2" t="n">
-        <v>50</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>68</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>18</v>
+        <v>-32</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
-          <t>-0.0%</t>
+          <t>-0.05%</t>
         </is>
       </c>
       <c r="S2" s="2" t="n">
-        <v>1.36</v>
+        <v>1.43</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>998</v>
-      </c>
+        <v>948</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>26.12.2024</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>1 - 2</t>
+        </is>
+      </c>
+      <c r="J3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="2" t="n"/>
+      <c r="O3" s="2" t="n"/>
+      <c r="P3" s="2" t="n"/>
+      <c r="Q3" s="2" t="n"/>
+      <c r="R3" s="2" t="n"/>
+      <c r="S3" s="2" t="n"/>
+      <c r="T3" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -724,7 +779,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
@@ -779,14 +834,14 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
integrate add button feature
</commit_message>
<xml_diff>
--- a/app/placed_bets.xlsx
+++ b/app/placed_bets.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -140,6 +140,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -592,7 +595,7 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
-      <c r="L1" s="3" t="inlineStr">
+      <c r="L1" s="12" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
@@ -676,7 +679,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J2" s="3" t="n">
+      <c r="J2" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="n"/>
@@ -748,7 +751,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J3" s="3" t="n">
+      <c r="J3" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K3" s="2" t="n"/>
@@ -800,7 +803,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="n"/>
@@ -852,7 +855,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J5" s="3" t="n">
+      <c r="J5" s="12" t="n">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n"/>

</xml_diff>

<commit_message>
fix file names until Feb 2025
</commit_message>
<xml_diff>
--- a/app/placed_bets.xlsx
+++ b/app/placed_bets.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -140,6 +140,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -519,7 +528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,7 +537,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="17" customWidth="1" min="1" max="1"/>
-    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="26" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
@@ -601,12 +610,12 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
-      <c r="L1" s="13" t="inlineStr">
+      <c r="L1" s="16" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="M1" s="12" t="inlineStr">
+      <c r="M1" s="15" t="inlineStr">
         <is>
           <t>Losses</t>
         </is>
@@ -685,27 +694,27 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J2" s="13" t="n">
+      <c r="J2" s="16" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>62.5</v>
+        <v>66.67</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>370</v>
+        <v>570</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>335</v>
+        <v>531</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>-35</v>
+        <v>-39</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
@@ -713,10 +722,10 @@
         </is>
       </c>
       <c r="S2" s="2" t="n">
-        <v>1.44</v>
+        <v>1.4</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>965</v>
+        <v>961</v>
       </c>
     </row>
     <row r="3">
@@ -757,7 +766,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J3" s="12" t="n">
+      <c r="J3" s="15" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="n"/>
@@ -809,7 +818,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J4" s="13" t="n">
+      <c r="J4" s="16" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="n"/>
@@ -861,7 +870,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J5" s="13" t="n">
+      <c r="J5" s="16" t="n">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n"/>
@@ -913,7 +922,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J6" s="13" t="n">
+      <c r="J6" s="16" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="n"/>
@@ -965,7 +974,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J7" s="12" t="n">
+      <c r="J7" s="15" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="2" t="n"/>
@@ -1017,7 +1026,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J8" s="13" t="n">
+      <c r="J8" s="16" t="n">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="n"/>
@@ -1069,7 +1078,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J9" s="12" t="n">
+      <c r="J9" s="15" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="2" t="n"/>
@@ -1082,6 +1091,214 @@
       <c r="R9" s="2" t="n"/>
       <c r="S9" s="2" t="n"/>
       <c r="T9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>05.01.2025</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>Olympique Marseille</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>Le Havre</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>66.5</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="I10" s="2" t="inlineStr">
+        <is>
+          <t>5 - 1</t>
+        </is>
+      </c>
+      <c r="J10" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="n"/>
+      <c r="L10" s="2" t="n"/>
+      <c r="M10" s="2" t="n"/>
+      <c r="N10" s="2" t="n"/>
+      <c r="O10" s="2" t="n"/>
+      <c r="P10" s="2" t="n"/>
+      <c r="Q10" s="2" t="n"/>
+      <c r="R10" s="2" t="n"/>
+      <c r="S10" s="2" t="n"/>
+      <c r="T10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>10.01.2025</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Como</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>IX</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="I11" s="2" t="inlineStr">
+        <is>
+          <t>1 - 1</t>
+        </is>
+      </c>
+      <c r="J11" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2" t="n"/>
+      <c r="L11" s="2" t="n"/>
+      <c r="M11" s="2" t="n"/>
+      <c r="N11" s="2" t="n"/>
+      <c r="O11" s="2" t="n"/>
+      <c r="P11" s="2" t="n"/>
+      <c r="Q11" s="2" t="n"/>
+      <c r="R11" s="2" t="n"/>
+      <c r="S11" s="2" t="n"/>
+      <c r="T11" s="2" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>11.01.2025</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>AC Milan</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="I12" s="2" t="inlineStr">
+        <is>
+          <t>1 - 1</t>
+        </is>
+      </c>
+      <c r="J12" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2" t="n"/>
+      <c r="L12" s="2" t="n"/>
+      <c r="M12" s="2" t="n"/>
+      <c r="N12" s="2" t="n"/>
+      <c r="O12" s="2" t="n"/>
+      <c r="P12" s="2" t="n"/>
+      <c r="Q12" s="2" t="n"/>
+      <c r="R12" s="2" t="n"/>
+      <c r="S12" s="2" t="n"/>
+      <c r="T12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>12.01.2025</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>Venezia</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Inter Milan</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="I13" s="2" t="inlineStr">
+        <is>
+          <t>0 - 1</t>
+        </is>
+      </c>
+      <c r="J13" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="n"/>
+      <c r="L13" s="2" t="n"/>
+      <c r="M13" s="2" t="n"/>
+      <c r="N13" s="2" t="n"/>
+      <c r="O13" s="2" t="n"/>
+      <c r="P13" s="2" t="n"/>
+      <c r="Q13" s="2" t="n"/>
+      <c r="R13" s="2" t="n"/>
+      <c r="S13" s="2" t="n"/>
+      <c r="T13" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1407,14 +1624,14 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1425,10 +1642,10 @@
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
@@ -1461,14 +1678,14 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
@@ -1551,14 +1768,14 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add first 16 bets
</commit_message>
<xml_diff>
--- a/app/placed_bets.xlsx
+++ b/app/placed_bets.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -152,6 +152,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -528,7 +540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -538,7 +550,7 @@
   <cols>
     <col width="17" customWidth="1" min="1" max="1"/>
     <col width="26" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="24" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
@@ -610,12 +622,12 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
-      <c r="L1" s="16" t="inlineStr">
+      <c r="L1" s="21" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="M1" s="15" t="inlineStr">
+      <c r="M1" s="18" t="inlineStr">
         <is>
           <t>Losses</t>
         </is>
@@ -694,38 +706,38 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J2" s="16" t="n">
+      <c r="J2" s="21" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>66.67</v>
+        <v>68.75</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>570</v>
+        <v>770</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>531</v>
+        <v>715.5</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>-39</v>
+        <v>-54.5</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
-          <t>-0.04%</t>
+          <t>-0.05%</t>
         </is>
       </c>
       <c r="S2" s="2" t="n">
-        <v>1.4</v>
+        <v>1.35</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>961</v>
+        <v>945.5</v>
       </c>
     </row>
     <row r="3">
@@ -766,7 +778,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J3" s="15" t="n">
+      <c r="J3" s="18" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="n"/>
@@ -818,7 +830,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J4" s="16" t="n">
+      <c r="J4" s="21" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="n"/>
@@ -870,7 +882,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J5" s="16" t="n">
+      <c r="J5" s="21" t="n">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n"/>
@@ -922,7 +934,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J6" s="16" t="n">
+      <c r="J6" s="21" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="n"/>
@@ -974,7 +986,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J7" s="15" t="n">
+      <c r="J7" s="18" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="2" t="n"/>
@@ -1026,7 +1038,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J8" s="16" t="n">
+      <c r="J8" s="21" t="n">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="n"/>
@@ -1078,7 +1090,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J9" s="15" t="n">
+      <c r="J9" s="18" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="2" t="n"/>
@@ -1130,7 +1142,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J10" s="16" t="n">
+      <c r="J10" s="21" t="n">
         <v>1</v>
       </c>
       <c r="K10" s="2" t="n"/>
@@ -1182,7 +1194,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J11" s="16" t="n">
+      <c r="J11" s="21" t="n">
         <v>1</v>
       </c>
       <c r="K11" s="2" t="n"/>
@@ -1234,7 +1246,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J12" s="15" t="n">
+      <c r="J12" s="18" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="2" t="n"/>
@@ -1286,7 +1298,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J13" s="16" t="n">
+      <c r="J13" s="21" t="n">
         <v>1</v>
       </c>
       <c r="K13" s="2" t="n"/>
@@ -1299,6 +1311,214 @@
       <c r="R13" s="2" t="n"/>
       <c r="S13" s="2" t="n"/>
       <c r="T13" s="2" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>12.01.2025</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>Atletico Madrid</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>Osasuna</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>66.5</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="I14" s="2" t="inlineStr">
+        <is>
+          <t>1 - 0</t>
+        </is>
+      </c>
+      <c r="J14" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="n"/>
+      <c r="L14" s="2" t="n"/>
+      <c r="M14" s="2" t="n"/>
+      <c r="N14" s="2" t="n"/>
+      <c r="O14" s="2" t="n"/>
+      <c r="P14" s="2" t="n"/>
+      <c r="Q14" s="2" t="n"/>
+      <c r="R14" s="2" t="n"/>
+      <c r="S14" s="2" t="n"/>
+      <c r="T14" s="2" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>12.01.2025</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>Verona</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I15" s="2" t="inlineStr">
+        <is>
+          <t>2 - 0</t>
+        </is>
+      </c>
+      <c r="J15" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2" t="n"/>
+      <c r="L15" s="2" t="n"/>
+      <c r="M15" s="2" t="n"/>
+      <c r="N15" s="2" t="n"/>
+      <c r="O15" s="2" t="n"/>
+      <c r="P15" s="2" t="n"/>
+      <c r="Q15" s="2" t="n"/>
+      <c r="R15" s="2" t="n"/>
+      <c r="S15" s="2" t="n"/>
+      <c r="T15" s="2" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>12.01.2025</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>Saint Etienne</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>55.50000000000001</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>5.500000000000007</v>
+      </c>
+      <c r="I16" s="2" t="inlineStr">
+        <is>
+          <t>2 - 1</t>
+        </is>
+      </c>
+      <c r="J16" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="n"/>
+      <c r="L16" s="2" t="n"/>
+      <c r="M16" s="2" t="n"/>
+      <c r="N16" s="2" t="n"/>
+      <c r="O16" s="2" t="n"/>
+      <c r="P16" s="2" t="n"/>
+      <c r="Q16" s="2" t="n"/>
+      <c r="R16" s="2" t="n"/>
+      <c r="S16" s="2" t="n"/>
+      <c r="T16" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>14.01.2025</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>Holstein Kiel</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>Borussia Dortmund</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>56.99999999999999</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>6.999999999999993</v>
+      </c>
+      <c r="I17" s="2" t="inlineStr">
+        <is>
+          <t>4 - 2</t>
+        </is>
+      </c>
+      <c r="J17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2" t="n"/>
+      <c r="L17" s="2" t="n"/>
+      <c r="M17" s="2" t="n"/>
+      <c r="N17" s="2" t="n"/>
+      <c r="O17" s="2" t="n"/>
+      <c r="P17" s="2" t="n"/>
+      <c r="Q17" s="2" t="n"/>
+      <c r="R17" s="2" t="n"/>
+      <c r="S17" s="2" t="n"/>
+      <c r="T17" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1444,14 +1664,14 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
@@ -1534,14 +1754,14 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1696,10 +1916,10 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
@@ -1822,14 +2042,14 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add 7 more bets - until 2025_01_19_2
</commit_message>
<xml_diff>
--- a/app/placed_bets.xlsx
+++ b/app/placed_bets.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -173,6 +173,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -540,7 +561,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,7 +584,7 @@
     <col width="13" customWidth="1" min="13" max="13"/>
     <col width="21" customWidth="1" min="14" max="14"/>
     <col width="15" customWidth="1" min="15" max="15"/>
-    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="13" customWidth="1" min="16" max="16"/>
     <col width="13" customWidth="1" min="17" max="17"/>
     <col width="13" customWidth="1" min="18" max="18"/>
     <col width="19" customWidth="1" min="19" max="19"/>
@@ -622,12 +643,12 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
-      <c r="L1" s="21" t="inlineStr">
+      <c r="L1" s="27" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="M1" s="18" t="inlineStr">
+      <c r="M1" s="26" t="inlineStr">
         <is>
           <t>Losses</t>
         </is>
@@ -706,38 +727,38 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J2" s="21" t="n">
+      <c r="J2" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>68.75</v>
+        <v>65.22</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>770</v>
+        <v>1420</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>715.5</v>
+        <v>1195.5</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>-54.5</v>
+        <v>-224.5</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
-          <t>-0.05%</t>
+          <t>-0.22%</t>
         </is>
       </c>
       <c r="S2" s="2" t="n">
-        <v>1.35</v>
+        <v>1.36</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>945.5</v>
+        <v>775.5</v>
       </c>
     </row>
     <row r="3">
@@ -778,7 +799,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J3" s="18" t="n">
+      <c r="J3" s="26" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="n"/>
@@ -830,7 +851,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J4" s="21" t="n">
+      <c r="J4" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="n"/>
@@ -882,7 +903,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J5" s="21" t="n">
+      <c r="J5" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n"/>
@@ -934,7 +955,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J6" s="21" t="n">
+      <c r="J6" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="n"/>
@@ -986,7 +1007,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J7" s="18" t="n">
+      <c r="J7" s="26" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="2" t="n"/>
@@ -1038,7 +1059,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J8" s="21" t="n">
+      <c r="J8" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="n"/>
@@ -1090,7 +1111,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J9" s="18" t="n">
+      <c r="J9" s="26" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="2" t="n"/>
@@ -1142,7 +1163,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J10" s="21" t="n">
+      <c r="J10" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K10" s="2" t="n"/>
@@ -1194,7 +1215,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J11" s="21" t="n">
+      <c r="J11" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K11" s="2" t="n"/>
@@ -1246,7 +1267,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J12" s="18" t="n">
+      <c r="J12" s="26" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="2" t="n"/>
@@ -1298,7 +1319,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J13" s="21" t="n">
+      <c r="J13" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K13" s="2" t="n"/>
@@ -1350,7 +1371,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J14" s="21" t="n">
+      <c r="J14" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="2" t="n"/>
@@ -1402,7 +1423,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J15" s="21" t="n">
+      <c r="J15" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K15" s="2" t="n"/>
@@ -1454,7 +1475,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J16" s="21" t="n">
+      <c r="J16" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K16" s="2" t="n"/>
@@ -1506,7 +1527,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J17" s="18" t="n">
+      <c r="J17" s="26" t="n">
         <v>0</v>
       </c>
       <c r="K17" s="2" t="n"/>
@@ -1519,6 +1540,370 @@
       <c r="R17" s="2" t="n"/>
       <c r="S17" s="2" t="n"/>
       <c r="T17" s="2" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>15.01.2025</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>Bayern Munchen</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>Hoffenheim</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>56.99999999999999</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>6.999999999999993</v>
+      </c>
+      <c r="I18" s="2" t="inlineStr">
+        <is>
+          <t>5 - 0</t>
+        </is>
+      </c>
+      <c r="J18" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2" t="n"/>
+      <c r="L18" s="2" t="n"/>
+      <c r="M18" s="2" t="n"/>
+      <c r="N18" s="2" t="n"/>
+      <c r="O18" s="2" t="n"/>
+      <c r="P18" s="2" t="n"/>
+      <c r="Q18" s="2" t="n"/>
+      <c r="R18" s="2" t="n"/>
+      <c r="S18" s="2" t="n"/>
+      <c r="T18" s="2" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>17.01.2025</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>Montpellier</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>Monaco</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>15.99999999999999</v>
+      </c>
+      <c r="I19" s="2" t="inlineStr">
+        <is>
+          <t>2 - 1</t>
+        </is>
+      </c>
+      <c r="J19" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2" t="n"/>
+      <c r="L19" s="2" t="n"/>
+      <c r="M19" s="2" t="n"/>
+      <c r="N19" s="2" t="n"/>
+      <c r="O19" s="2" t="n"/>
+      <c r="P19" s="2" t="n"/>
+      <c r="Q19" s="2" t="n"/>
+      <c r="R19" s="2" t="n"/>
+      <c r="S19" s="2" t="n"/>
+      <c r="T19" s="2" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>18.01.2025</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>Bochum</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I20" s="2" t="inlineStr">
+        <is>
+          <t>3 - 3</t>
+        </is>
+      </c>
+      <c r="J20" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2" t="n"/>
+      <c r="L20" s="2" t="n"/>
+      <c r="M20" s="2" t="n"/>
+      <c r="N20" s="2" t="n"/>
+      <c r="O20" s="2" t="n"/>
+      <c r="P20" s="2" t="n"/>
+      <c r="Q20" s="2" t="n"/>
+      <c r="R20" s="2" t="n"/>
+      <c r="S20" s="2" t="n"/>
+      <c r="T20" s="2" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>18.01.2025</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>Leganes</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>Atletico Madrid</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>151</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="I21" s="2" t="inlineStr">
+        <is>
+          <t>1 - 0</t>
+        </is>
+      </c>
+      <c r="J21" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="n"/>
+      <c r="L21" s="2" t="n"/>
+      <c r="M21" s="2" t="n"/>
+      <c r="N21" s="2" t="n"/>
+      <c r="O21" s="2" t="n"/>
+      <c r="P21" s="2" t="n"/>
+      <c r="Q21" s="2" t="n"/>
+      <c r="R21" s="2" t="n"/>
+      <c r="S21" s="2" t="n"/>
+      <c r="T21" s="2" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>18.01.2025</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>Lens</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>173</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="I22" s="2" t="inlineStr">
+        <is>
+          <t>1 - 2</t>
+        </is>
+      </c>
+      <c r="J22" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" s="2" t="n"/>
+      <c r="L22" s="2" t="n"/>
+      <c r="M22" s="2" t="n"/>
+      <c r="N22" s="2" t="n"/>
+      <c r="O22" s="2" t="n"/>
+      <c r="P22" s="2" t="n"/>
+      <c r="Q22" s="2" t="n"/>
+      <c r="R22" s="2" t="n"/>
+      <c r="S22" s="2" t="n"/>
+      <c r="T22" s="2" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>18.01.2025</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>Getafe</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>153</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="I23" s="2" t="inlineStr">
+        <is>
+          <t>1 - 1</t>
+        </is>
+      </c>
+      <c r="J23" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2" t="n"/>
+      <c r="L23" s="2" t="n"/>
+      <c r="M23" s="2" t="n"/>
+      <c r="N23" s="2" t="n"/>
+      <c r="O23" s="2" t="n"/>
+      <c r="P23" s="2" t="n"/>
+      <c r="Q23" s="2" t="n"/>
+      <c r="R23" s="2" t="n"/>
+      <c r="S23" s="2" t="n"/>
+      <c r="T23" s="2" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>19.01.2025</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>Las Palmas</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I24" s="2" t="inlineStr">
+        <is>
+          <t>4 - 1</t>
+        </is>
+      </c>
+      <c r="J24" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2" t="n"/>
+      <c r="L24" s="2" t="n"/>
+      <c r="M24" s="2" t="n"/>
+      <c r="N24" s="2" t="n"/>
+      <c r="O24" s="2" t="n"/>
+      <c r="P24" s="2" t="n"/>
+      <c r="Q24" s="2" t="n"/>
+      <c r="R24" s="2" t="n"/>
+      <c r="S24" s="2" t="n"/>
+      <c r="T24" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1664,14 +2049,14 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -1682,14 +2067,14 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1700,10 +2085,10 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
@@ -1736,14 +2121,14 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
@@ -1808,14 +2193,14 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
@@ -2006,14 +2391,14 @@
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -2042,10 +2427,10 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
populate until March 2025
</commit_message>
<xml_diff>
--- a/app/placed_bets.xlsx
+++ b/app/placed_bets.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -245,6 +245,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -612,7 +630,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T57"/>
+  <dimension ref="A1:T65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -622,7 +640,7 @@
   <cols>
     <col width="17" customWidth="1" min="1" max="1"/>
     <col width="26" customWidth="1" min="2" max="2"/>
-    <col width="24" customWidth="1" min="3" max="3"/>
+    <col width="26" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
@@ -694,12 +712,12 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
-      <c r="L1" s="44" t="inlineStr">
+      <c r="L1" s="51" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="M1" s="42" t="inlineStr">
+      <c r="M1" s="50" t="inlineStr">
         <is>
           <t>Losses</t>
         </is>
@@ -778,38 +796,38 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J2" s="44" t="n">
+      <c r="J2" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>71.43000000000001</v>
+        <v>70.31</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>4720</v>
+        <v>5520</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>4433.5</v>
+        <v>5067.5</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>-286.5</v>
+        <v>-452.5</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
-          <t>-0.29%</t>
+          <t>-0.45%</t>
         </is>
       </c>
       <c r="S2" s="2" t="n">
         <v>1.33</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>713.5</v>
+        <v>547.5</v>
       </c>
     </row>
     <row r="3">
@@ -850,7 +868,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J3" s="42" t="n">
+      <c r="J3" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="n"/>
@@ -902,7 +920,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J4" s="44" t="n">
+      <c r="J4" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="n"/>
@@ -954,7 +972,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J5" s="44" t="n">
+      <c r="J5" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n"/>
@@ -1006,7 +1024,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J6" s="44" t="n">
+      <c r="J6" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="n"/>
@@ -1058,7 +1076,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J7" s="42" t="n">
+      <c r="J7" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="2" t="n"/>
@@ -1110,7 +1128,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J8" s="44" t="n">
+      <c r="J8" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="n"/>
@@ -1162,7 +1180,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J9" s="42" t="n">
+      <c r="J9" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="2" t="n"/>
@@ -1214,7 +1232,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J10" s="44" t="n">
+      <c r="J10" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K10" s="2" t="n"/>
@@ -1266,7 +1284,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J11" s="44" t="n">
+      <c r="J11" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K11" s="2" t="n"/>
@@ -1318,7 +1336,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J12" s="42" t="n">
+      <c r="J12" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="2" t="n"/>
@@ -1370,7 +1388,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J13" s="44" t="n">
+      <c r="J13" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K13" s="2" t="n"/>
@@ -1422,7 +1440,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J14" s="44" t="n">
+      <c r="J14" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="2" t="n"/>
@@ -1474,7 +1492,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J15" s="44" t="n">
+      <c r="J15" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K15" s="2" t="n"/>
@@ -1526,7 +1544,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J16" s="44" t="n">
+      <c r="J16" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K16" s="2" t="n"/>
@@ -1578,7 +1596,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J17" s="42" t="n">
+      <c r="J17" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K17" s="2" t="n"/>
@@ -1630,7 +1648,7 @@
           <t>5 - 0</t>
         </is>
       </c>
-      <c r="J18" s="44" t="n">
+      <c r="J18" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K18" s="2" t="n"/>
@@ -1682,7 +1700,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J19" s="42" t="n">
+      <c r="J19" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="2" t="n"/>
@@ -1734,7 +1752,7 @@
           <t>3 - 3</t>
         </is>
       </c>
-      <c r="J20" s="44" t="n">
+      <c r="J20" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K20" s="2" t="n"/>
@@ -1786,7 +1804,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J21" s="42" t="n">
+      <c r="J21" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K21" s="2" t="n"/>
@@ -1838,7 +1856,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J22" s="44" t="n">
+      <c r="J22" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K22" s="2" t="n"/>
@@ -1890,7 +1908,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J23" s="42" t="n">
+      <c r="J23" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K23" s="2" t="n"/>
@@ -1942,7 +1960,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J24" s="44" t="n">
+      <c r="J24" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K24" s="2" t="n"/>
@@ -1994,7 +2012,7 @@
           <t>0 - 6</t>
         </is>
       </c>
-      <c r="J25" s="44" t="n">
+      <c r="J25" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K25" s="2" t="n"/>
@@ -2046,7 +2064,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J26" s="44" t="n">
+      <c r="J26" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K26" s="2" t="n"/>
@@ -2098,7 +2116,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J27" s="44" t="n">
+      <c r="J27" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K27" s="2" t="n"/>
@@ -2150,7 +2168,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J28" s="44" t="n">
+      <c r="J28" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K28" s="2" t="n"/>
@@ -2202,7 +2220,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J29" s="42" t="n">
+      <c r="J29" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K29" s="2" t="n"/>
@@ -2254,7 +2272,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J30" s="44" t="n">
+      <c r="J30" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K30" s="2" t="n"/>
@@ -2306,7 +2324,7 @@
           <t>0 - 4</t>
         </is>
       </c>
-      <c r="J31" s="44" t="n">
+      <c r="J31" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K31" s="2" t="n"/>
@@ -2358,7 +2376,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J32" s="44" t="n">
+      <c r="J32" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K32" s="2" t="n"/>
@@ -2410,7 +2428,7 @@
           <t>2 - 5</t>
         </is>
       </c>
-      <c r="J33" s="44" t="n">
+      <c r="J33" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K33" s="2" t="n"/>
@@ -2462,7 +2480,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J34" s="42" t="n">
+      <c r="J34" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K34" s="2" t="n"/>
@@ -2514,7 +2532,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J35" s="44" t="n">
+      <c r="J35" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K35" s="2" t="n"/>
@@ -2566,7 +2584,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J36" s="44" t="n">
+      <c r="J36" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K36" s="2" t="n"/>
@@ -2618,7 +2636,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J37" s="44" t="n">
+      <c r="J37" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K37" s="2" t="n"/>
@@ -2670,7 +2688,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J38" s="44" t="n">
+      <c r="J38" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K38" s="2" t="n"/>
@@ -2722,7 +2740,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J39" s="44" t="n">
+      <c r="J39" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K39" s="2" t="n"/>
@@ -2774,7 +2792,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J40" s="44" t="n">
+      <c r="J40" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K40" s="2" t="n"/>
@@ -2826,7 +2844,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J41" s="44" t="n">
+      <c r="J41" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K41" s="2" t="n"/>
@@ -2878,7 +2896,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J42" s="44" t="n">
+      <c r="J42" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K42" s="2" t="n"/>
@@ -2930,7 +2948,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J43" s="42" t="n">
+      <c r="J43" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K43" s="2" t="n"/>
@@ -2982,7 +3000,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J44" s="44" t="n">
+      <c r="J44" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K44" s="2" t="n"/>
@@ -3034,7 +3052,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J45" s="42" t="n">
+      <c r="J45" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K45" s="2" t="n"/>
@@ -3086,7 +3104,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J46" s="44" t="n">
+      <c r="J46" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K46" s="2" t="n"/>
@@ -3138,7 +3156,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J47" s="44" t="n">
+      <c r="J47" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K47" s="2" t="n"/>
@@ -3190,7 +3208,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J48" s="42" t="n">
+      <c r="J48" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K48" s="2" t="n"/>
@@ -3242,7 +3260,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J49" s="44" t="n">
+      <c r="J49" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K49" s="2" t="n"/>
@@ -3294,7 +3312,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J50" s="44" t="n">
+      <c r="J50" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K50" s="2" t="n"/>
@@ -3346,7 +3364,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J51" s="44" t="n">
+      <c r="J51" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K51" s="2" t="n"/>
@@ -3398,7 +3416,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J52" s="42" t="n">
+      <c r="J52" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K52" s="2" t="n"/>
@@ -3450,7 +3468,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J53" s="44" t="n">
+      <c r="J53" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K53" s="2" t="n"/>
@@ -3502,7 +3520,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J54" s="42" t="n">
+      <c r="J54" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K54" s="2" t="n"/>
@@ -3554,7 +3572,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J55" s="42" t="n">
+      <c r="J55" s="50" t="n">
         <v>0</v>
       </c>
       <c r="K55" s="2" t="n"/>
@@ -3606,7 +3624,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J56" s="44" t="n">
+      <c r="J56" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K56" s="2" t="n"/>
@@ -3658,7 +3676,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J57" s="44" t="n">
+      <c r="J57" s="51" t="n">
         <v>1</v>
       </c>
       <c r="K57" s="2" t="n"/>
@@ -3671,6 +3689,422 @@
       <c r="R57" s="2" t="n"/>
       <c r="S57" s="2" t="n"/>
       <c r="T57" s="2" t="n"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="inlineStr">
+        <is>
+          <t>22.02.2025</t>
+        </is>
+      </c>
+      <c r="B58" s="2" t="inlineStr">
+        <is>
+          <t>Las Palmas</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="F58" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G58" s="2" t="n">
+        <v>124</v>
+      </c>
+      <c r="H58" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="I58" s="2" t="inlineStr">
+        <is>
+          <t>0 - 2</t>
+        </is>
+      </c>
+      <c r="J58" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="K58" s="2" t="n"/>
+      <c r="L58" s="2" t="n"/>
+      <c r="M58" s="2" t="n"/>
+      <c r="N58" s="2" t="n"/>
+      <c r="O58" s="2" t="n"/>
+      <c r="P58" s="2" t="n"/>
+      <c r="Q58" s="2" t="n"/>
+      <c r="R58" s="2" t="n"/>
+      <c r="S58" s="2" t="n"/>
+      <c r="T58" s="2" t="n"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="inlineStr">
+        <is>
+          <t>22.02.2025</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="inlineStr">
+        <is>
+          <t>Auxerre</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="inlineStr">
+        <is>
+          <t>Olympique Marseille</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="F59" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G59" s="2" t="n">
+        <v>155</v>
+      </c>
+      <c r="H59" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="I59" s="2" t="inlineStr">
+        <is>
+          <t>3 - 0</t>
+        </is>
+      </c>
+      <c r="J59" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" s="2" t="n"/>
+      <c r="L59" s="2" t="n"/>
+      <c r="M59" s="2" t="n"/>
+      <c r="N59" s="2" t="n"/>
+      <c r="O59" s="2" t="n"/>
+      <c r="P59" s="2" t="n"/>
+      <c r="Q59" s="2" t="n"/>
+      <c r="R59" s="2" t="n"/>
+      <c r="S59" s="2" t="n"/>
+      <c r="T59" s="2" t="n"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>23.02.2025</t>
+        </is>
+      </c>
+      <c r="B60" s="2" t="inlineStr">
+        <is>
+          <t>Como</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="F60" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G60" s="2" t="n">
+        <v>132</v>
+      </c>
+      <c r="H60" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="I60" s="2" t="inlineStr">
+        <is>
+          <t>2 - 1</t>
+        </is>
+      </c>
+      <c r="J60" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" s="2" t="n"/>
+      <c r="L60" s="2" t="n"/>
+      <c r="M60" s="2" t="n"/>
+      <c r="N60" s="2" t="n"/>
+      <c r="O60" s="2" t="n"/>
+      <c r="P60" s="2" t="n"/>
+      <c r="Q60" s="2" t="n"/>
+      <c r="R60" s="2" t="n"/>
+      <c r="S60" s="2" t="n"/>
+      <c r="T60" s="2" t="n"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="inlineStr">
+        <is>
+          <t>23.02.2025</t>
+        </is>
+      </c>
+      <c r="B61" s="2" t="inlineStr">
+        <is>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="inlineStr">
+        <is>
+          <t>Heidenheim</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="F61" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G61" s="2" t="n">
+        <v>132</v>
+      </c>
+      <c r="H61" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="I61" s="2" t="inlineStr">
+        <is>
+          <t>2 - 2</t>
+        </is>
+      </c>
+      <c r="J61" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" s="2" t="n"/>
+      <c r="L61" s="2" t="n"/>
+      <c r="M61" s="2" t="n"/>
+      <c r="N61" s="2" t="n"/>
+      <c r="O61" s="2" t="n"/>
+      <c r="P61" s="2" t="n"/>
+      <c r="Q61" s="2" t="n"/>
+      <c r="R61" s="2" t="n"/>
+      <c r="S61" s="2" t="n"/>
+      <c r="T61" s="2" t="n"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>23.02.2025</t>
+        </is>
+      </c>
+      <c r="B62" s="2" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="inlineStr">
+        <is>
+          <t>Girona</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="F62" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G62" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="H62" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I62" s="2" t="inlineStr">
+        <is>
+          <t>2 - 0</t>
+        </is>
+      </c>
+      <c r="J62" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="K62" s="2" t="n"/>
+      <c r="L62" s="2" t="n"/>
+      <c r="M62" s="2" t="n"/>
+      <c r="N62" s="2" t="n"/>
+      <c r="O62" s="2" t="n"/>
+      <c r="P62" s="2" t="n"/>
+      <c r="Q62" s="2" t="n"/>
+      <c r="R62" s="2" t="n"/>
+      <c r="S62" s="2" t="n"/>
+      <c r="T62" s="2" t="n"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="inlineStr">
+        <is>
+          <t>23.02.2025</t>
+        </is>
+      </c>
+      <c r="B63" s="2" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="C63" s="2" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="F63" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G63" s="2" t="n">
+        <v>124</v>
+      </c>
+      <c r="H63" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="I63" s="2" t="inlineStr">
+        <is>
+          <t>0 - 1</t>
+        </is>
+      </c>
+      <c r="J63" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="K63" s="2" t="n"/>
+      <c r="L63" s="2" t="n"/>
+      <c r="M63" s="2" t="n"/>
+      <c r="N63" s="2" t="n"/>
+      <c r="O63" s="2" t="n"/>
+      <c r="P63" s="2" t="n"/>
+      <c r="Q63" s="2" t="n"/>
+      <c r="R63" s="2" t="n"/>
+      <c r="S63" s="2" t="n"/>
+      <c r="T63" s="2" t="n"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>25.02.2025</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="inlineStr">
+        <is>
+          <t>Southampton</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F64" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G64" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I64" s="2" t="inlineStr">
+        <is>
+          <t>4 - 0</t>
+        </is>
+      </c>
+      <c r="J64" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="K64" s="2" t="n"/>
+      <c r="L64" s="2" t="n"/>
+      <c r="M64" s="2" t="n"/>
+      <c r="N64" s="2" t="n"/>
+      <c r="O64" s="2" t="n"/>
+      <c r="P64" s="2" t="n"/>
+      <c r="Q64" s="2" t="n"/>
+      <c r="R64" s="2" t="n"/>
+      <c r="S64" s="2" t="n"/>
+      <c r="T64" s="2" t="n"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="inlineStr">
+        <is>
+          <t>28.02.2025</t>
+        </is>
+      </c>
+      <c r="B65" s="2" t="inlineStr">
+        <is>
+          <t>Monaco</t>
+        </is>
+      </c>
+      <c r="C65" s="2" t="inlineStr">
+        <is>
+          <t>Reims</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="F65" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G65" s="2" t="n">
+        <v>136</v>
+      </c>
+      <c r="H65" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="I65" s="2" t="inlineStr">
+        <is>
+          <t>3 - 0</t>
+        </is>
+      </c>
+      <c r="J65" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="K65" s="2" t="n"/>
+      <c r="L65" s="2" t="n"/>
+      <c r="M65" s="2" t="n"/>
+      <c r="N65" s="2" t="n"/>
+      <c r="O65" s="2" t="n"/>
+      <c r="P65" s="2" t="n"/>
+      <c r="Q65" s="2" t="n"/>
+      <c r="R65" s="2" t="n"/>
+      <c r="S65" s="2" t="n"/>
+      <c r="T65" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3744,14 +4178,14 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>25.0%</t>
         </is>
       </c>
     </row>
@@ -3834,14 +4268,14 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>2</v>
-      </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>66.67%</t>
+          <t>75.0%</t>
         </is>
       </c>
     </row>
@@ -3852,14 +4286,14 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>4</v>
-      </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>80.0%</t>
+          <t>83.33%</t>
         </is>
       </c>
     </row>
@@ -3960,14 +4394,14 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -4032,10 +4466,10 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
@@ -4068,14 +4502,14 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>66.67%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -4140,14 +4574,14 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>66.67%</t>
         </is>
       </c>
     </row>
@@ -4158,14 +4592,14 @@
         </is>
       </c>
       <c r="B26" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>1</v>
-      </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>66.67%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add Bayern bet (2-0 lead but lost) - 8.03.2025
</commit_message>
<xml_diff>
--- a/app/placed_bets.xlsx
+++ b/app/placed_bets.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -254,6 +254,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -630,7 +639,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T65"/>
+  <dimension ref="A1:T70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -712,12 +721,12 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
-      <c r="L1" s="51" t="inlineStr">
+      <c r="L1" s="54" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="M1" s="50" t="inlineStr">
+      <c r="M1" s="53" t="inlineStr">
         <is>
           <t>Losses</t>
         </is>
@@ -796,27 +805,27 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J2" s="51" t="n">
+      <c r="J2" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>70.31</v>
+        <v>71.01000000000001</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>5520</v>
+        <v>5970</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>5067.5</v>
+        <v>5518.5</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>-452.5</v>
+        <v>-451.5</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
@@ -827,7 +836,7 @@
         <v>1.33</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>547.5</v>
+        <v>548.5</v>
       </c>
     </row>
     <row r="3">
@@ -868,7 +877,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J3" s="50" t="n">
+      <c r="J3" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="n"/>
@@ -920,7 +929,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J4" s="51" t="n">
+      <c r="J4" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="n"/>
@@ -972,7 +981,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J5" s="51" t="n">
+      <c r="J5" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n"/>
@@ -1024,7 +1033,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J6" s="51" t="n">
+      <c r="J6" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="n"/>
@@ -1076,7 +1085,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J7" s="50" t="n">
+      <c r="J7" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="2" t="n"/>
@@ -1128,7 +1137,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J8" s="51" t="n">
+      <c r="J8" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="n"/>
@@ -1180,7 +1189,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J9" s="50" t="n">
+      <c r="J9" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="2" t="n"/>
@@ -1232,7 +1241,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J10" s="51" t="n">
+      <c r="J10" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K10" s="2" t="n"/>
@@ -1284,7 +1293,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J11" s="51" t="n">
+      <c r="J11" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K11" s="2" t="n"/>
@@ -1336,7 +1345,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J12" s="50" t="n">
+      <c r="J12" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="2" t="n"/>
@@ -1388,7 +1397,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J13" s="51" t="n">
+      <c r="J13" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K13" s="2" t="n"/>
@@ -1440,7 +1449,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J14" s="51" t="n">
+      <c r="J14" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="2" t="n"/>
@@ -1492,7 +1501,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J15" s="51" t="n">
+      <c r="J15" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K15" s="2" t="n"/>
@@ -1544,7 +1553,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J16" s="51" t="n">
+      <c r="J16" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K16" s="2" t="n"/>
@@ -1596,7 +1605,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J17" s="50" t="n">
+      <c r="J17" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K17" s="2" t="n"/>
@@ -1648,7 +1657,7 @@
           <t>5 - 0</t>
         </is>
       </c>
-      <c r="J18" s="51" t="n">
+      <c r="J18" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K18" s="2" t="n"/>
@@ -1700,7 +1709,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J19" s="50" t="n">
+      <c r="J19" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="2" t="n"/>
@@ -1752,7 +1761,7 @@
           <t>3 - 3</t>
         </is>
       </c>
-      <c r="J20" s="51" t="n">
+      <c r="J20" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K20" s="2" t="n"/>
@@ -1804,7 +1813,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J21" s="50" t="n">
+      <c r="J21" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K21" s="2" t="n"/>
@@ -1856,7 +1865,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J22" s="51" t="n">
+      <c r="J22" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K22" s="2" t="n"/>
@@ -1908,7 +1917,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J23" s="50" t="n">
+      <c r="J23" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K23" s="2" t="n"/>
@@ -1960,7 +1969,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J24" s="51" t="n">
+      <c r="J24" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K24" s="2" t="n"/>
@@ -2012,7 +2021,7 @@
           <t>0 - 6</t>
         </is>
       </c>
-      <c r="J25" s="51" t="n">
+      <c r="J25" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K25" s="2" t="n"/>
@@ -2064,7 +2073,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J26" s="51" t="n">
+      <c r="J26" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K26" s="2" t="n"/>
@@ -2116,7 +2125,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J27" s="51" t="n">
+      <c r="J27" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K27" s="2" t="n"/>
@@ -2168,7 +2177,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J28" s="51" t="n">
+      <c r="J28" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K28" s="2" t="n"/>
@@ -2220,7 +2229,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J29" s="50" t="n">
+      <c r="J29" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K29" s="2" t="n"/>
@@ -2272,7 +2281,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J30" s="51" t="n">
+      <c r="J30" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K30" s="2" t="n"/>
@@ -2324,7 +2333,7 @@
           <t>0 - 4</t>
         </is>
       </c>
-      <c r="J31" s="51" t="n">
+      <c r="J31" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K31" s="2" t="n"/>
@@ -2376,7 +2385,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J32" s="51" t="n">
+      <c r="J32" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K32" s="2" t="n"/>
@@ -2428,7 +2437,7 @@
           <t>2 - 5</t>
         </is>
       </c>
-      <c r="J33" s="51" t="n">
+      <c r="J33" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K33" s="2" t="n"/>
@@ -2480,7 +2489,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J34" s="50" t="n">
+      <c r="J34" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K34" s="2" t="n"/>
@@ -2532,7 +2541,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J35" s="51" t="n">
+      <c r="J35" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K35" s="2" t="n"/>
@@ -2584,7 +2593,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J36" s="51" t="n">
+      <c r="J36" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K36" s="2" t="n"/>
@@ -2636,7 +2645,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J37" s="51" t="n">
+      <c r="J37" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K37" s="2" t="n"/>
@@ -2688,7 +2697,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J38" s="51" t="n">
+      <c r="J38" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K38" s="2" t="n"/>
@@ -2740,7 +2749,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J39" s="51" t="n">
+      <c r="J39" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K39" s="2" t="n"/>
@@ -2792,7 +2801,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J40" s="51" t="n">
+      <c r="J40" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K40" s="2" t="n"/>
@@ -2844,7 +2853,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J41" s="51" t="n">
+      <c r="J41" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K41" s="2" t="n"/>
@@ -2896,7 +2905,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J42" s="51" t="n">
+      <c r="J42" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K42" s="2" t="n"/>
@@ -2948,7 +2957,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J43" s="50" t="n">
+      <c r="J43" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K43" s="2" t="n"/>
@@ -3000,7 +3009,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J44" s="51" t="n">
+      <c r="J44" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K44" s="2" t="n"/>
@@ -3052,7 +3061,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J45" s="50" t="n">
+      <c r="J45" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K45" s="2" t="n"/>
@@ -3104,7 +3113,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J46" s="51" t="n">
+      <c r="J46" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K46" s="2" t="n"/>
@@ -3156,7 +3165,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J47" s="51" t="n">
+      <c r="J47" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K47" s="2" t="n"/>
@@ -3208,7 +3217,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J48" s="50" t="n">
+      <c r="J48" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K48" s="2" t="n"/>
@@ -3260,7 +3269,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J49" s="51" t="n">
+      <c r="J49" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K49" s="2" t="n"/>
@@ -3312,7 +3321,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J50" s="51" t="n">
+      <c r="J50" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K50" s="2" t="n"/>
@@ -3364,7 +3373,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J51" s="51" t="n">
+      <c r="J51" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K51" s="2" t="n"/>
@@ -3416,7 +3425,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J52" s="50" t="n">
+      <c r="J52" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K52" s="2" t="n"/>
@@ -3468,7 +3477,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J53" s="51" t="n">
+      <c r="J53" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K53" s="2" t="n"/>
@@ -3520,7 +3529,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J54" s="50" t="n">
+      <c r="J54" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K54" s="2" t="n"/>
@@ -3572,7 +3581,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J55" s="50" t="n">
+      <c r="J55" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K55" s="2" t="n"/>
@@ -3624,7 +3633,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J56" s="51" t="n">
+      <c r="J56" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K56" s="2" t="n"/>
@@ -3676,7 +3685,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J57" s="51" t="n">
+      <c r="J57" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K57" s="2" t="n"/>
@@ -3728,7 +3737,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J58" s="51" t="n">
+      <c r="J58" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K58" s="2" t="n"/>
@@ -3780,7 +3789,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J59" s="50" t="n">
+      <c r="J59" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K59" s="2" t="n"/>
@@ -3832,7 +3841,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J60" s="50" t="n">
+      <c r="J60" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K60" s="2" t="n"/>
@@ -3884,7 +3893,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J61" s="50" t="n">
+      <c r="J61" s="53" t="n">
         <v>0</v>
       </c>
       <c r="K61" s="2" t="n"/>
@@ -3936,7 +3945,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J62" s="51" t="n">
+      <c r="J62" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K62" s="2" t="n"/>
@@ -3988,7 +3997,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J63" s="51" t="n">
+      <c r="J63" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K63" s="2" t="n"/>
@@ -4040,7 +4049,7 @@
           <t>4 - 0</t>
         </is>
       </c>
-      <c r="J64" s="51" t="n">
+      <c r="J64" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K64" s="2" t="n"/>
@@ -4092,7 +4101,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J65" s="51" t="n">
+      <c r="J65" s="54" t="n">
         <v>1</v>
       </c>
       <c r="K65" s="2" t="n"/>
@@ -4105,6 +4114,266 @@
       <c r="R65" s="2" t="n"/>
       <c r="S65" s="2" t="n"/>
       <c r="T65" s="2" t="n"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="inlineStr">
+        <is>
+          <t>01.03.2025</t>
+        </is>
+      </c>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>Betis</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="F66" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G66" s="2" t="n">
+        <v>127</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I66" s="2" t="inlineStr">
+        <is>
+          <t>2 - 1</t>
+        </is>
+      </c>
+      <c r="J66" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" s="2" t="n"/>
+      <c r="L66" s="2" t="n"/>
+      <c r="M66" s="2" t="n"/>
+      <c r="N66" s="2" t="n"/>
+      <c r="O66" s="2" t="n"/>
+      <c r="P66" s="2" t="n"/>
+      <c r="Q66" s="2" t="n"/>
+      <c r="R66" s="2" t="n"/>
+      <c r="S66" s="2" t="n"/>
+      <c r="T66" s="2" t="n"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="inlineStr">
+        <is>
+          <t>02.03.2025</t>
+        </is>
+      </c>
+      <c r="B67" s="2" t="inlineStr">
+        <is>
+          <t>Olympique Lyon</t>
+        </is>
+      </c>
+      <c r="C67" s="2" t="inlineStr">
+        <is>
+          <t>Brest</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>1X</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F67" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G67" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="H67" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I67" s="2" t="inlineStr">
+        <is>
+          <t>2 - 1</t>
+        </is>
+      </c>
+      <c r="J67" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="K67" s="2" t="n"/>
+      <c r="L67" s="2" t="n"/>
+      <c r="M67" s="2" t="n"/>
+      <c r="N67" s="2" t="n"/>
+      <c r="O67" s="2" t="n"/>
+      <c r="P67" s="2" t="n"/>
+      <c r="Q67" s="2" t="n"/>
+      <c r="R67" s="2" t="n"/>
+      <c r="S67" s="2" t="n"/>
+      <c r="T67" s="2" t="n"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="inlineStr">
+        <is>
+          <t>02.03.2025</t>
+        </is>
+      </c>
+      <c r="B68" s="2" t="inlineStr">
+        <is>
+          <t>Olympique Marseille</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="inlineStr">
+        <is>
+          <t>Nantes</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E68" s="2" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="F68" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G68" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="H68" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="I68" s="2" t="inlineStr">
+        <is>
+          <t>2 - 0</t>
+        </is>
+      </c>
+      <c r="J68" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="K68" s="2" t="n"/>
+      <c r="L68" s="2" t="n"/>
+      <c r="M68" s="2" t="n"/>
+      <c r="N68" s="2" t="n"/>
+      <c r="O68" s="2" t="n"/>
+      <c r="P68" s="2" t="n"/>
+      <c r="Q68" s="2" t="n"/>
+      <c r="R68" s="2" t="n"/>
+      <c r="S68" s="2" t="n"/>
+      <c r="T68" s="2" t="n"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="inlineStr">
+        <is>
+          <t>03.03.2025</t>
+        </is>
+      </c>
+      <c r="B69" s="2" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="inlineStr">
+        <is>
+          <t>Verona</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="F69" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G69" s="2" t="n">
+        <v>134</v>
+      </c>
+      <c r="H69" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="I69" s="2" t="inlineStr">
+        <is>
+          <t>2 - 0</t>
+        </is>
+      </c>
+      <c r="J69" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="K69" s="2" t="n"/>
+      <c r="L69" s="2" t="n"/>
+      <c r="M69" s="2" t="n"/>
+      <c r="N69" s="2" t="n"/>
+      <c r="O69" s="2" t="n"/>
+      <c r="P69" s="2" t="n"/>
+      <c r="Q69" s="2" t="n"/>
+      <c r="R69" s="2" t="n"/>
+      <c r="S69" s="2" t="n"/>
+      <c r="T69" s="2" t="n"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="inlineStr">
+        <is>
+          <t>08.03.2025</t>
+        </is>
+      </c>
+      <c r="B70" s="2" t="inlineStr">
+        <is>
+          <t>Bayern Munchen</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="inlineStr">
+        <is>
+          <t>Bochum</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F70" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G70" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="H70" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I70" s="2" t="inlineStr">
+        <is>
+          <t>2 - 3</t>
+        </is>
+      </c>
+      <c r="J70" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="K70" s="2" t="n"/>
+      <c r="L70" s="2" t="n"/>
+      <c r="M70" s="2" t="n"/>
+      <c r="N70" s="2" t="n"/>
+      <c r="O70" s="2" t="n"/>
+      <c r="P70" s="2" t="n"/>
+      <c r="Q70" s="2" t="n"/>
+      <c r="R70" s="2" t="n"/>
+      <c r="S70" s="2" t="n"/>
+      <c r="T70" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4286,14 +4555,14 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>83.33%</t>
+          <t>71.43%</t>
         </is>
       </c>
     </row>
@@ -4322,10 +4591,10 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
@@ -4466,10 +4735,10 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
@@ -4552,18 +4821,18 @@
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>Lyon</t>
+          <t>Olympique Lyon</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -4574,14 +4843,14 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C25" s="2" t="n">
-        <v>2</v>
-      </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>66.67%</t>
+          <t>75.0%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
manually add Stuttgart game on 8.03.2025
</commit_message>
<xml_diff>
--- a/app/placed_bets.xlsx
+++ b/app/placed_bets.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -254,6 +254,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -639,7 +648,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T70"/>
+  <dimension ref="A1:T73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -653,8 +662,8 @@
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="24" customWidth="1" min="7" max="7"/>
-    <col width="24" customWidth="1" min="8" max="8"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
     <col width="13" customWidth="1" min="9" max="9"/>
     <col width="14" customWidth="1" min="10" max="10"/>
     <col width="11" customWidth="1" min="11" max="11"/>
@@ -721,12 +730,12 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
-      <c r="L1" s="54" t="inlineStr">
+      <c r="L1" s="57" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="M1" s="53" t="inlineStr">
+      <c r="M1" s="56" t="inlineStr">
         <is>
           <t>Losses</t>
         </is>
@@ -805,38 +814,38 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J2" s="54" t="n">
+      <c r="J2" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>71.01000000000001</v>
+        <v>70.83</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>5970</v>
+        <v>6270</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>5518.5</v>
+        <v>5747.5</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>-451.5</v>
+        <v>-522.5</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
-          <t>-0.45%</t>
+          <t>-0.52%</t>
         </is>
       </c>
       <c r="S2" s="2" t="n">
         <v>1.33</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>548.5</v>
+        <v>477.5</v>
       </c>
     </row>
     <row r="3">
@@ -877,7 +886,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J3" s="53" t="n">
+      <c r="J3" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="n"/>
@@ -929,7 +938,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J4" s="54" t="n">
+      <c r="J4" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="n"/>
@@ -981,7 +990,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J5" s="54" t="n">
+      <c r="J5" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n"/>
@@ -1033,7 +1042,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J6" s="54" t="n">
+      <c r="J6" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="n"/>
@@ -1085,7 +1094,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J7" s="53" t="n">
+      <c r="J7" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="2" t="n"/>
@@ -1137,7 +1146,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J8" s="54" t="n">
+      <c r="J8" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="n"/>
@@ -1189,7 +1198,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J9" s="53" t="n">
+      <c r="J9" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="2" t="n"/>
@@ -1241,7 +1250,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J10" s="54" t="n">
+      <c r="J10" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K10" s="2" t="n"/>
@@ -1293,7 +1302,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J11" s="54" t="n">
+      <c r="J11" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K11" s="2" t="n"/>
@@ -1345,7 +1354,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J12" s="53" t="n">
+      <c r="J12" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="2" t="n"/>
@@ -1397,7 +1406,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J13" s="54" t="n">
+      <c r="J13" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K13" s="2" t="n"/>
@@ -1449,7 +1458,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J14" s="54" t="n">
+      <c r="J14" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="2" t="n"/>
@@ -1501,7 +1510,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J15" s="54" t="n">
+      <c r="J15" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K15" s="2" t="n"/>
@@ -1553,7 +1562,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J16" s="54" t="n">
+      <c r="J16" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K16" s="2" t="n"/>
@@ -1605,7 +1614,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J17" s="53" t="n">
+      <c r="J17" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K17" s="2" t="n"/>
@@ -1657,7 +1666,7 @@
           <t>5 - 0</t>
         </is>
       </c>
-      <c r="J18" s="54" t="n">
+      <c r="J18" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K18" s="2" t="n"/>
@@ -1709,7 +1718,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J19" s="53" t="n">
+      <c r="J19" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="2" t="n"/>
@@ -1761,7 +1770,7 @@
           <t>3 - 3</t>
         </is>
       </c>
-      <c r="J20" s="54" t="n">
+      <c r="J20" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K20" s="2" t="n"/>
@@ -1813,7 +1822,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J21" s="53" t="n">
+      <c r="J21" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K21" s="2" t="n"/>
@@ -1865,7 +1874,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J22" s="54" t="n">
+      <c r="J22" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K22" s="2" t="n"/>
@@ -1917,7 +1926,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J23" s="53" t="n">
+      <c r="J23" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K23" s="2" t="n"/>
@@ -1969,7 +1978,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J24" s="54" t="n">
+      <c r="J24" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K24" s="2" t="n"/>
@@ -2021,7 +2030,7 @@
           <t>0 - 6</t>
         </is>
       </c>
-      <c r="J25" s="54" t="n">
+      <c r="J25" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K25" s="2" t="n"/>
@@ -2073,7 +2082,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J26" s="54" t="n">
+      <c r="J26" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K26" s="2" t="n"/>
@@ -2125,7 +2134,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J27" s="54" t="n">
+      <c r="J27" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K27" s="2" t="n"/>
@@ -2177,7 +2186,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J28" s="54" t="n">
+      <c r="J28" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K28" s="2" t="n"/>
@@ -2229,7 +2238,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J29" s="53" t="n">
+      <c r="J29" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K29" s="2" t="n"/>
@@ -2281,7 +2290,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J30" s="54" t="n">
+      <c r="J30" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K30" s="2" t="n"/>
@@ -2333,7 +2342,7 @@
           <t>0 - 4</t>
         </is>
       </c>
-      <c r="J31" s="54" t="n">
+      <c r="J31" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K31" s="2" t="n"/>
@@ -2385,7 +2394,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J32" s="54" t="n">
+      <c r="J32" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K32" s="2" t="n"/>
@@ -2437,7 +2446,7 @@
           <t>2 - 5</t>
         </is>
       </c>
-      <c r="J33" s="54" t="n">
+      <c r="J33" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K33" s="2" t="n"/>
@@ -2489,7 +2498,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J34" s="53" t="n">
+      <c r="J34" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K34" s="2" t="n"/>
@@ -2541,7 +2550,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J35" s="54" t="n">
+      <c r="J35" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K35" s="2" t="n"/>
@@ -2593,7 +2602,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J36" s="54" t="n">
+      <c r="J36" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K36" s="2" t="n"/>
@@ -2645,7 +2654,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J37" s="54" t="n">
+      <c r="J37" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K37" s="2" t="n"/>
@@ -2697,7 +2706,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J38" s="54" t="n">
+      <c r="J38" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K38" s="2" t="n"/>
@@ -2749,7 +2758,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J39" s="54" t="n">
+      <c r="J39" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K39" s="2" t="n"/>
@@ -2801,7 +2810,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J40" s="54" t="n">
+      <c r="J40" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K40" s="2" t="n"/>
@@ -2853,7 +2862,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J41" s="54" t="n">
+      <c r="J41" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K41" s="2" t="n"/>
@@ -2905,7 +2914,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J42" s="54" t="n">
+      <c r="J42" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K42" s="2" t="n"/>
@@ -2957,7 +2966,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J43" s="53" t="n">
+      <c r="J43" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K43" s="2" t="n"/>
@@ -3009,7 +3018,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J44" s="54" t="n">
+      <c r="J44" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K44" s="2" t="n"/>
@@ -3061,7 +3070,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J45" s="53" t="n">
+      <c r="J45" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K45" s="2" t="n"/>
@@ -3113,7 +3122,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J46" s="54" t="n">
+      <c r="J46" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K46" s="2" t="n"/>
@@ -3165,7 +3174,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J47" s="54" t="n">
+      <c r="J47" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K47" s="2" t="n"/>
@@ -3217,7 +3226,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J48" s="53" t="n">
+      <c r="J48" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K48" s="2" t="n"/>
@@ -3269,7 +3278,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J49" s="54" t="n">
+      <c r="J49" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K49" s="2" t="n"/>
@@ -3321,7 +3330,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J50" s="54" t="n">
+      <c r="J50" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K50" s="2" t="n"/>
@@ -3373,7 +3382,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J51" s="54" t="n">
+      <c r="J51" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K51" s="2" t="n"/>
@@ -3425,7 +3434,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J52" s="53" t="n">
+      <c r="J52" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K52" s="2" t="n"/>
@@ -3477,7 +3486,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J53" s="54" t="n">
+      <c r="J53" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K53" s="2" t="n"/>
@@ -3529,7 +3538,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J54" s="53" t="n">
+      <c r="J54" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K54" s="2" t="n"/>
@@ -3581,7 +3590,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J55" s="53" t="n">
+      <c r="J55" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K55" s="2" t="n"/>
@@ -3633,7 +3642,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J56" s="54" t="n">
+      <c r="J56" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K56" s="2" t="n"/>
@@ -3685,7 +3694,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J57" s="54" t="n">
+      <c r="J57" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K57" s="2" t="n"/>
@@ -3737,7 +3746,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J58" s="54" t="n">
+      <c r="J58" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K58" s="2" t="n"/>
@@ -3789,7 +3798,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J59" s="53" t="n">
+      <c r="J59" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K59" s="2" t="n"/>
@@ -3841,7 +3850,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J60" s="53" t="n">
+      <c r="J60" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K60" s="2" t="n"/>
@@ -3893,7 +3902,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J61" s="53" t="n">
+      <c r="J61" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K61" s="2" t="n"/>
@@ -3945,7 +3954,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J62" s="54" t="n">
+      <c r="J62" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K62" s="2" t="n"/>
@@ -3997,7 +4006,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J63" s="54" t="n">
+      <c r="J63" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K63" s="2" t="n"/>
@@ -4049,7 +4058,7 @@
           <t>4 - 0</t>
         </is>
       </c>
-      <c r="J64" s="54" t="n">
+      <c r="J64" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K64" s="2" t="n"/>
@@ -4101,7 +4110,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J65" s="54" t="n">
+      <c r="J65" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K65" s="2" t="n"/>
@@ -4153,7 +4162,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J66" s="53" t="n">
+      <c r="J66" s="56" t="n">
         <v>0</v>
       </c>
       <c r="K66" s="2" t="n"/>
@@ -4205,7 +4214,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J67" s="54" t="n">
+      <c r="J67" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K67" s="2" t="n"/>
@@ -4257,7 +4266,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J68" s="54" t="n">
+      <c r="J68" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K68" s="2" t="n"/>
@@ -4309,7 +4318,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J69" s="54" t="n">
+      <c r="J69" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K69" s="2" t="n"/>
@@ -4361,7 +4370,7 @@
           <t>2 - 3</t>
         </is>
       </c>
-      <c r="J70" s="54" t="n">
+      <c r="J70" s="57" t="n">
         <v>1</v>
       </c>
       <c r="K70" s="2" t="n"/>
@@ -4374,6 +4383,162 @@
       <c r="R70" s="2" t="n"/>
       <c r="S70" s="2" t="n"/>
       <c r="T70" s="2" t="n"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="inlineStr">
+        <is>
+          <t>08.03.2025</t>
+        </is>
+      </c>
+      <c r="B71" s="2" t="inlineStr">
+        <is>
+          <t>Bayer Leverkusen</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="inlineStr">
+        <is>
+          <t>Werder Bremen</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="F71" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G71" s="2" t="n">
+        <v>135</v>
+      </c>
+      <c r="H71" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="I71" s="2" t="inlineStr">
+        <is>
+          <t>0 - 2</t>
+        </is>
+      </c>
+      <c r="J71" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" s="2" t="n"/>
+      <c r="L71" s="2" t="n"/>
+      <c r="M71" s="2" t="n"/>
+      <c r="N71" s="2" t="n"/>
+      <c r="O71" s="2" t="n"/>
+      <c r="P71" s="2" t="n"/>
+      <c r="Q71" s="2" t="n"/>
+      <c r="R71" s="2" t="n"/>
+      <c r="S71" s="2" t="n"/>
+      <c r="T71" s="2" t="n"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="inlineStr">
+        <is>
+          <t>08.03.2025</t>
+        </is>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>Holstein Kiel</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="inlineStr">
+        <is>
+          <t>Stuttgart</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E72" s="2" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="F72" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G72" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="H72" s="2" t="n">
+        <v>15.99999999999999</v>
+      </c>
+      <c r="I72" s="2" t="inlineStr">
+        <is>
+          <t>2 - 2</t>
+        </is>
+      </c>
+      <c r="J72" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="K72" s="2" t="n"/>
+      <c r="L72" s="2" t="n"/>
+      <c r="M72" s="2" t="n"/>
+      <c r="N72" s="2" t="n"/>
+      <c r="O72" s="2" t="n"/>
+      <c r="P72" s="2" t="n"/>
+      <c r="Q72" s="2" t="n"/>
+      <c r="R72" s="2" t="n"/>
+      <c r="S72" s="2" t="n"/>
+      <c r="T72" s="2" t="n"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="inlineStr">
+        <is>
+          <t>08.03.2025</t>
+        </is>
+      </c>
+      <c r="B73" s="2" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="C73" s="2" t="inlineStr">
+        <is>
+          <t>Southampton</t>
+        </is>
+      </c>
+      <c r="D73" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E73" s="2" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="F73" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G73" s="2" t="n">
+        <v>113</v>
+      </c>
+      <c r="H73" s="2" t="n">
+        <v>12.99999999999999</v>
+      </c>
+      <c r="I73" s="2" t="inlineStr">
+        <is>
+          <t>3 - 1</t>
+        </is>
+      </c>
+      <c r="J73" s="57" t="n">
+        <v>1</v>
+      </c>
+      <c r="K73" s="2" t="n"/>
+      <c r="L73" s="2" t="n"/>
+      <c r="M73" s="2" t="n"/>
+      <c r="N73" s="2" t="n"/>
+      <c r="O73" s="2" t="n"/>
+      <c r="P73" s="2" t="n"/>
+      <c r="Q73" s="2" t="n"/>
+      <c r="R73" s="2" t="n"/>
+      <c r="S73" s="2" t="n"/>
+      <c r="T73" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4465,10 +4630,10 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
@@ -4573,14 +4738,14 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>75.0%</t>
         </is>
       </c>
     </row>
@@ -4681,14 +4846,14 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add Liverpool game on 2.04.025
</commit_message>
<xml_diff>
--- a/app/placed_bets.xlsx
+++ b/app/placed_bets.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -308,6 +308,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -690,7 +711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T89"/>
+  <dimension ref="A1:T97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -772,7 +793,7 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
-      <c r="L1" s="71" t="inlineStr">
+      <c r="L1" s="78" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
@@ -856,38 +877,38 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J2" s="71" t="n">
+      <c r="J2" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>26</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>70.45</v>
+        <v>72.92</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>7420</v>
+        <v>7820</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>6728.5</v>
+        <v>7186</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>-691.5</v>
+        <v>-634</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
-          <t>-0.69%</t>
+          <t>-0.63%</t>
         </is>
       </c>
       <c r="S2" s="2" t="n">
         <v>1.34</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>308.5</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3">
@@ -980,7 +1001,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J4" s="71" t="n">
+      <c r="J4" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="n"/>
@@ -1032,7 +1053,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J5" s="71" t="n">
+      <c r="J5" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n"/>
@@ -1084,7 +1105,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J6" s="71" t="n">
+      <c r="J6" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="n"/>
@@ -1188,7 +1209,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J8" s="71" t="n">
+      <c r="J8" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="n"/>
@@ -1292,7 +1313,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J10" s="71" t="n">
+      <c r="J10" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K10" s="2" t="n"/>
@@ -1344,7 +1365,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J11" s="71" t="n">
+      <c r="J11" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K11" s="2" t="n"/>
@@ -1448,7 +1469,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J13" s="71" t="n">
+      <c r="J13" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K13" s="2" t="n"/>
@@ -1500,7 +1521,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J14" s="71" t="n">
+      <c r="J14" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="2" t="n"/>
@@ -1552,7 +1573,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J15" s="71" t="n">
+      <c r="J15" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K15" s="2" t="n"/>
@@ -1604,7 +1625,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J16" s="71" t="n">
+      <c r="J16" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K16" s="2" t="n"/>
@@ -1708,7 +1729,7 @@
           <t>5 - 0</t>
         </is>
       </c>
-      <c r="J18" s="71" t="n">
+      <c r="J18" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K18" s="2" t="n"/>
@@ -1812,7 +1833,7 @@
           <t>3 - 3</t>
         </is>
       </c>
-      <c r="J20" s="71" t="n">
+      <c r="J20" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K20" s="2" t="n"/>
@@ -1916,7 +1937,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J22" s="71" t="n">
+      <c r="J22" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K22" s="2" t="n"/>
@@ -2020,7 +2041,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J24" s="71" t="n">
+      <c r="J24" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K24" s="2" t="n"/>
@@ -2072,7 +2093,7 @@
           <t>0 - 6</t>
         </is>
       </c>
-      <c r="J25" s="71" t="n">
+      <c r="J25" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K25" s="2" t="n"/>
@@ -2124,7 +2145,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J26" s="71" t="n">
+      <c r="J26" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K26" s="2" t="n"/>
@@ -2176,7 +2197,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J27" s="71" t="n">
+      <c r="J27" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K27" s="2" t="n"/>
@@ -2228,7 +2249,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J28" s="71" t="n">
+      <c r="J28" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K28" s="2" t="n"/>
@@ -2332,7 +2353,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J30" s="71" t="n">
+      <c r="J30" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K30" s="2" t="n"/>
@@ -2384,7 +2405,7 @@
           <t>0 - 4</t>
         </is>
       </c>
-      <c r="J31" s="71" t="n">
+      <c r="J31" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K31" s="2" t="n"/>
@@ -2436,7 +2457,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J32" s="71" t="n">
+      <c r="J32" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K32" s="2" t="n"/>
@@ -2488,7 +2509,7 @@
           <t>2 - 5</t>
         </is>
       </c>
-      <c r="J33" s="71" t="n">
+      <c r="J33" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K33" s="2" t="n"/>
@@ -2592,7 +2613,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J35" s="71" t="n">
+      <c r="J35" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K35" s="2" t="n"/>
@@ -2644,7 +2665,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J36" s="71" t="n">
+      <c r="J36" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K36" s="2" t="n"/>
@@ -2696,7 +2717,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J37" s="71" t="n">
+      <c r="J37" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K37" s="2" t="n"/>
@@ -2748,7 +2769,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J38" s="71" t="n">
+      <c r="J38" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K38" s="2" t="n"/>
@@ -2800,7 +2821,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J39" s="71" t="n">
+      <c r="J39" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K39" s="2" t="n"/>
@@ -2852,7 +2873,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J40" s="71" t="n">
+      <c r="J40" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K40" s="2" t="n"/>
@@ -2904,7 +2925,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J41" s="71" t="n">
+      <c r="J41" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K41" s="2" t="n"/>
@@ -2956,7 +2977,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J42" s="71" t="n">
+      <c r="J42" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K42" s="2" t="n"/>
@@ -3060,7 +3081,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J44" s="71" t="n">
+      <c r="J44" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K44" s="2" t="n"/>
@@ -3164,7 +3185,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J46" s="71" t="n">
+      <c r="J46" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K46" s="2" t="n"/>
@@ -3216,7 +3237,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J47" s="71" t="n">
+      <c r="J47" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K47" s="2" t="n"/>
@@ -3320,7 +3341,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J49" s="71" t="n">
+      <c r="J49" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K49" s="2" t="n"/>
@@ -3372,7 +3393,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J50" s="71" t="n">
+      <c r="J50" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K50" s="2" t="n"/>
@@ -3424,7 +3445,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J51" s="71" t="n">
+      <c r="J51" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K51" s="2" t="n"/>
@@ -3528,7 +3549,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J53" s="71" t="n">
+      <c r="J53" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K53" s="2" t="n"/>
@@ -3684,7 +3705,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J56" s="71" t="n">
+      <c r="J56" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K56" s="2" t="n"/>
@@ -3736,7 +3757,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J57" s="71" t="n">
+      <c r="J57" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K57" s="2" t="n"/>
@@ -3788,7 +3809,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J58" s="71" t="n">
+      <c r="J58" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K58" s="2" t="n"/>
@@ -3996,7 +4017,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J62" s="71" t="n">
+      <c r="J62" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K62" s="2" t="n"/>
@@ -4048,7 +4069,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J63" s="71" t="n">
+      <c r="J63" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K63" s="2" t="n"/>
@@ -4100,7 +4121,7 @@
           <t>4 - 0</t>
         </is>
       </c>
-      <c r="J64" s="71" t="n">
+      <c r="J64" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K64" s="2" t="n"/>
@@ -4152,7 +4173,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J65" s="71" t="n">
+      <c r="J65" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K65" s="2" t="n"/>
@@ -4256,7 +4277,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J67" s="71" t="n">
+      <c r="J67" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K67" s="2" t="n"/>
@@ -4308,7 +4329,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J68" s="71" t="n">
+      <c r="J68" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K68" s="2" t="n"/>
@@ -4360,7 +4381,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J69" s="71" t="n">
+      <c r="J69" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K69" s="2" t="n"/>
@@ -4412,7 +4433,7 @@
           <t>2 - 3</t>
         </is>
       </c>
-      <c r="J70" s="71" t="n">
+      <c r="J70" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K70" s="2" t="n"/>
@@ -4516,7 +4537,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J72" s="71" t="n">
+      <c r="J72" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K72" s="2" t="n"/>
@@ -4568,7 +4589,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J73" s="71" t="n">
+      <c r="J73" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K73" s="2" t="n"/>
@@ -4620,7 +4641,7 @@
           <t>1 - 4</t>
         </is>
       </c>
-      <c r="J74" s="71" t="n">
+      <c r="J74" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K74" s="2" t="n"/>
@@ -4672,7 +4693,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J75" s="71" t="n">
+      <c r="J75" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K75" s="2" t="n"/>
@@ -4724,7 +4745,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J76" s="71" t="n">
+      <c r="J76" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K76" s="2" t="n"/>
@@ -4880,7 +4901,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J79" s="71" t="n">
+      <c r="J79" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K79" s="2" t="n"/>
@@ -4984,7 +5005,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J81" s="71" t="n">
+      <c r="J81" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K81" s="2" t="n"/>
@@ -5036,7 +5057,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J82" s="71" t="n">
+      <c r="J82" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K82" s="2" t="n"/>
@@ -5192,7 +5213,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J85" s="71" t="n">
+      <c r="J85" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K85" s="2" t="n"/>
@@ -5244,7 +5265,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J86" s="71" t="n">
+      <c r="J86" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K86" s="2" t="n"/>
@@ -5296,7 +5317,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J87" s="71" t="n">
+      <c r="J87" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K87" s="2" t="n"/>
@@ -5348,7 +5369,7 @@
           <t>1 - 3</t>
         </is>
       </c>
-      <c r="J88" s="71" t="n">
+      <c r="J88" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K88" s="2" t="n"/>
@@ -5400,7 +5421,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J89" s="71" t="n">
+      <c r="J89" s="78" t="n">
         <v>1</v>
       </c>
       <c r="K89" s="2" t="n"/>
@@ -5413,6 +5434,422 @@
       <c r="R89" s="2" t="n"/>
       <c r="S89" s="2" t="n"/>
       <c r="T89" s="2" t="n"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="inlineStr">
+        <is>
+          <t>29.03.2025</t>
+        </is>
+      </c>
+      <c r="B90" s="2" t="inlineStr">
+        <is>
+          <t>Saint Etienne</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="F90" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G90" s="2" t="n">
+        <v>58.5</v>
+      </c>
+      <c r="H90" s="2" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="I90" s="2" t="inlineStr">
+        <is>
+          <t>1 - 6</t>
+        </is>
+      </c>
+      <c r="J90" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="K90" s="2" t="n"/>
+      <c r="L90" s="2" t="n"/>
+      <c r="M90" s="2" t="n"/>
+      <c r="N90" s="2" t="n"/>
+      <c r="O90" s="2" t="n"/>
+      <c r="P90" s="2" t="n"/>
+      <c r="Q90" s="2" t="n"/>
+      <c r="R90" s="2" t="n"/>
+      <c r="S90" s="2" t="n"/>
+      <c r="T90" s="2" t="n"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="inlineStr">
+        <is>
+          <t>29.03.2025</t>
+        </is>
+      </c>
+      <c r="B91" s="2" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="C91" s="2" t="inlineStr">
+        <is>
+          <t>Leganes</t>
+        </is>
+      </c>
+      <c r="D91" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E91" s="2" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="F91" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G91" s="2" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="H91" s="2" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="I91" s="2" t="inlineStr">
+        <is>
+          <t>3 - 2</t>
+        </is>
+      </c>
+      <c r="J91" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="K91" s="2" t="n"/>
+      <c r="L91" s="2" t="n"/>
+      <c r="M91" s="2" t="n"/>
+      <c r="N91" s="2" t="n"/>
+      <c r="O91" s="2" t="n"/>
+      <c r="P91" s="2" t="n"/>
+      <c r="Q91" s="2" t="n"/>
+      <c r="R91" s="2" t="n"/>
+      <c r="S91" s="2" t="n"/>
+      <c r="T91" s="2" t="n"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="inlineStr">
+        <is>
+          <t>01.04.2025</t>
+        </is>
+      </c>
+      <c r="B92" s="2" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="inlineStr">
+        <is>
+          <t>1X</t>
+        </is>
+      </c>
+      <c r="E92" s="2" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="F92" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G92" s="2" t="n">
+        <v>55.50000000000001</v>
+      </c>
+      <c r="H92" s="2" t="n">
+        <v>5.500000000000007</v>
+      </c>
+      <c r="I92" s="2" t="inlineStr">
+        <is>
+          <t>2 - 1</t>
+        </is>
+      </c>
+      <c r="J92" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="K92" s="2" t="n"/>
+      <c r="L92" s="2" t="n"/>
+      <c r="M92" s="2" t="n"/>
+      <c r="N92" s="2" t="n"/>
+      <c r="O92" s="2" t="n"/>
+      <c r="P92" s="2" t="n"/>
+      <c r="Q92" s="2" t="n"/>
+      <c r="R92" s="2" t="n"/>
+      <c r="S92" s="2" t="n"/>
+      <c r="T92" s="2" t="n"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="inlineStr">
+        <is>
+          <t>02.04.2025</t>
+        </is>
+      </c>
+      <c r="B93" s="2" t="inlineStr">
+        <is>
+          <t>Manchester City</t>
+        </is>
+      </c>
+      <c r="C93" s="2" t="inlineStr">
+        <is>
+          <t>Leicester</t>
+        </is>
+      </c>
+      <c r="D93" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E93" s="2" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="F93" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G93" s="2" t="n">
+        <v>60.5</v>
+      </c>
+      <c r="H93" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="I93" s="2" t="inlineStr">
+        <is>
+          <t>2 - 0</t>
+        </is>
+      </c>
+      <c r="J93" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="K93" s="2" t="n"/>
+      <c r="L93" s="2" t="n"/>
+      <c r="M93" s="2" t="n"/>
+      <c r="N93" s="2" t="n"/>
+      <c r="O93" s="2" t="n"/>
+      <c r="P93" s="2" t="n"/>
+      <c r="Q93" s="2" t="n"/>
+      <c r="R93" s="2" t="n"/>
+      <c r="S93" s="2" t="n"/>
+      <c r="T93" s="2" t="n"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="inlineStr">
+        <is>
+          <t>02.04.2025</t>
+        </is>
+      </c>
+      <c r="B94" s="2" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>IX</t>
+        </is>
+      </c>
+      <c r="E94" s="2" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="F94" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G94" s="2" t="n">
+        <v>55.50000000000001</v>
+      </c>
+      <c r="H94" s="2" t="n">
+        <v>5.500000000000007</v>
+      </c>
+      <c r="I94" s="2" t="inlineStr">
+        <is>
+          <t>1 - 0</t>
+        </is>
+      </c>
+      <c r="J94" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="K94" s="2" t="n"/>
+      <c r="L94" s="2" t="n"/>
+      <c r="M94" s="2" t="n"/>
+      <c r="N94" s="2" t="n"/>
+      <c r="O94" s="2" t="n"/>
+      <c r="P94" s="2" t="n"/>
+      <c r="Q94" s="2" t="n"/>
+      <c r="R94" s="2" t="n"/>
+      <c r="S94" s="2" t="n"/>
+      <c r="T94" s="2" t="n"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="inlineStr">
+        <is>
+          <t>04.04.2025</t>
+        </is>
+      </c>
+      <c r="B95" s="2" t="inlineStr">
+        <is>
+          <t>Augsburg</t>
+        </is>
+      </c>
+      <c r="C95" s="2" t="inlineStr">
+        <is>
+          <t>Bayern Munchen</t>
+        </is>
+      </c>
+      <c r="D95" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E95" s="2" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="F95" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G95" s="2" t="n">
+        <v>55.00000000000001</v>
+      </c>
+      <c r="H95" s="2" t="n">
+        <v>5.000000000000007</v>
+      </c>
+      <c r="I95" s="2" t="inlineStr">
+        <is>
+          <t>1 - 3</t>
+        </is>
+      </c>
+      <c r="J95" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="K95" s="2" t="n"/>
+      <c r="L95" s="2" t="n"/>
+      <c r="M95" s="2" t="n"/>
+      <c r="N95" s="2" t="n"/>
+      <c r="O95" s="2" t="n"/>
+      <c r="P95" s="2" t="n"/>
+      <c r="Q95" s="2" t="n"/>
+      <c r="R95" s="2" t="n"/>
+      <c r="S95" s="2" t="n"/>
+      <c r="T95" s="2" t="n"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="inlineStr">
+        <is>
+          <t>05.04.2025</t>
+        </is>
+      </c>
+      <c r="B96" s="2" t="inlineStr">
+        <is>
+          <t>Heidenheim</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="inlineStr">
+        <is>
+          <t>Bayer Leverkusen</t>
+        </is>
+      </c>
+      <c r="D96" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E96" s="2" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="F96" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G96" s="2" t="n">
+        <v>56.99999999999999</v>
+      </c>
+      <c r="H96" s="2" t="n">
+        <v>6.999999999999993</v>
+      </c>
+      <c r="I96" s="2" t="inlineStr">
+        <is>
+          <t>0 - 1</t>
+        </is>
+      </c>
+      <c r="J96" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="K96" s="2" t="n"/>
+      <c r="L96" s="2" t="n"/>
+      <c r="M96" s="2" t="n"/>
+      <c r="N96" s="2" t="n"/>
+      <c r="O96" s="2" t="n"/>
+      <c r="P96" s="2" t="n"/>
+      <c r="Q96" s="2" t="n"/>
+      <c r="R96" s="2" t="n"/>
+      <c r="S96" s="2" t="n"/>
+      <c r="T96" s="2" t="n"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="inlineStr">
+        <is>
+          <t>05.04.2025</t>
+        </is>
+      </c>
+      <c r="B97" s="2" t="inlineStr">
+        <is>
+          <t>Mainz</t>
+        </is>
+      </c>
+      <c r="C97" s="2" t="inlineStr">
+        <is>
+          <t>Holstein Kiel</t>
+        </is>
+      </c>
+      <c r="D97" s="2" t="inlineStr">
+        <is>
+          <t>IX</t>
+        </is>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="F97" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G97" s="2" t="n">
+        <v>56.00000000000001</v>
+      </c>
+      <c r="H97" s="2" t="n">
+        <v>6.000000000000007</v>
+      </c>
+      <c r="I97" s="2" t="inlineStr">
+        <is>
+          <t>1 - 1</t>
+        </is>
+      </c>
+      <c r="J97" s="78" t="n">
+        <v>1</v>
+      </c>
+      <c r="K97" s="2" t="n"/>
+      <c r="L97" s="2" t="n"/>
+      <c r="M97" s="2" t="n"/>
+      <c r="N97" s="2" t="n"/>
+      <c r="O97" s="2" t="n"/>
+      <c r="P97" s="2" t="n"/>
+      <c r="Q97" s="2" t="n"/>
+      <c r="R97" s="2" t="n"/>
+      <c r="S97" s="2" t="n"/>
+      <c r="T97" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5468,14 +5905,14 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>66.67%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -5504,10 +5941,10 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
@@ -5522,10 +5959,10 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
@@ -5594,14 +6031,14 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>75.0%</t>
+          <t>77.78%</t>
         </is>
       </c>
     </row>
@@ -5612,14 +6049,14 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>60.0%</t>
+          <t>66.67%</t>
         </is>
       </c>
     </row>
@@ -5630,14 +6067,14 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>3</v>
-      </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>75.0%</t>
+          <t>80.0%</t>
         </is>
       </c>
     </row>
@@ -5684,14 +6121,14 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
@@ -5936,14 +6373,14 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C28" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C28" s="2" t="n">
-        <v>5</v>
-      </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>83.33%</t>
+          <t>85.71%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add Man City match on 12.04.2025
</commit_message>
<xml_diff>
--- a/app/placed_bets.xlsx
+++ b/app/placed_bets.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -338,6 +338,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -711,7 +726,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T97"/>
+  <dimension ref="A1:T105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -793,12 +808,12 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
-      <c r="L1" s="78" t="inlineStr">
+      <c r="L1" s="83" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="M1" s="67" t="inlineStr">
+      <c r="M1" s="82" t="inlineStr">
         <is>
           <t>Losses</t>
         </is>
@@ -877,38 +892,38 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J2" s="78" t="n">
+      <c r="J2" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>72.92</v>
+        <v>73.08</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>7820</v>
+        <v>8220</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>7186</v>
+        <v>7527.5</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>-634</v>
+        <v>-692.5</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
-          <t>-0.63%</t>
+          <t>-0.69%</t>
         </is>
       </c>
       <c r="S2" s="2" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>366</v>
+        <v>307.5</v>
       </c>
     </row>
     <row r="3">
@@ -949,7 +964,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J3" s="67" t="n">
+      <c r="J3" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="n"/>
@@ -1001,7 +1016,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J4" s="78" t="n">
+      <c r="J4" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="n"/>
@@ -1053,7 +1068,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J5" s="78" t="n">
+      <c r="J5" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n"/>
@@ -1105,7 +1120,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J6" s="78" t="n">
+      <c r="J6" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="n"/>
@@ -1157,7 +1172,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J7" s="67" t="n">
+      <c r="J7" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="2" t="n"/>
@@ -1209,7 +1224,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J8" s="78" t="n">
+      <c r="J8" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="n"/>
@@ -1261,7 +1276,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J9" s="67" t="n">
+      <c r="J9" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="2" t="n"/>
@@ -1313,7 +1328,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J10" s="78" t="n">
+      <c r="J10" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K10" s="2" t="n"/>
@@ -1365,7 +1380,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J11" s="78" t="n">
+      <c r="J11" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K11" s="2" t="n"/>
@@ -1417,7 +1432,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J12" s="67" t="n">
+      <c r="J12" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="2" t="n"/>
@@ -1469,7 +1484,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J13" s="78" t="n">
+      <c r="J13" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K13" s="2" t="n"/>
@@ -1521,7 +1536,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J14" s="78" t="n">
+      <c r="J14" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="2" t="n"/>
@@ -1573,7 +1588,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J15" s="78" t="n">
+      <c r="J15" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K15" s="2" t="n"/>
@@ -1625,7 +1640,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J16" s="78" t="n">
+      <c r="J16" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K16" s="2" t="n"/>
@@ -1677,7 +1692,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J17" s="67" t="n">
+      <c r="J17" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K17" s="2" t="n"/>
@@ -1729,7 +1744,7 @@
           <t>5 - 0</t>
         </is>
       </c>
-      <c r="J18" s="78" t="n">
+      <c r="J18" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K18" s="2" t="n"/>
@@ -1781,7 +1796,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J19" s="67" t="n">
+      <c r="J19" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="2" t="n"/>
@@ -1833,7 +1848,7 @@
           <t>3 - 3</t>
         </is>
       </c>
-      <c r="J20" s="78" t="n">
+      <c r="J20" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K20" s="2" t="n"/>
@@ -1885,7 +1900,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J21" s="67" t="n">
+      <c r="J21" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K21" s="2" t="n"/>
@@ -1937,7 +1952,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J22" s="78" t="n">
+      <c r="J22" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K22" s="2" t="n"/>
@@ -1989,7 +2004,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J23" s="67" t="n">
+      <c r="J23" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K23" s="2" t="n"/>
@@ -2041,7 +2056,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J24" s="78" t="n">
+      <c r="J24" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K24" s="2" t="n"/>
@@ -2093,7 +2108,7 @@
           <t>0 - 6</t>
         </is>
       </c>
-      <c r="J25" s="78" t="n">
+      <c r="J25" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K25" s="2" t="n"/>
@@ -2145,7 +2160,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J26" s="78" t="n">
+      <c r="J26" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K26" s="2" t="n"/>
@@ -2197,7 +2212,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J27" s="78" t="n">
+      <c r="J27" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K27" s="2" t="n"/>
@@ -2249,7 +2264,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J28" s="78" t="n">
+      <c r="J28" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K28" s="2" t="n"/>
@@ -2301,7 +2316,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J29" s="67" t="n">
+      <c r="J29" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K29" s="2" t="n"/>
@@ -2353,7 +2368,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J30" s="78" t="n">
+      <c r="J30" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K30" s="2" t="n"/>
@@ -2405,7 +2420,7 @@
           <t>0 - 4</t>
         </is>
       </c>
-      <c r="J31" s="78" t="n">
+      <c r="J31" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K31" s="2" t="n"/>
@@ -2457,7 +2472,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J32" s="78" t="n">
+      <c r="J32" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K32" s="2" t="n"/>
@@ -2509,7 +2524,7 @@
           <t>2 - 5</t>
         </is>
       </c>
-      <c r="J33" s="78" t="n">
+      <c r="J33" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K33" s="2" t="n"/>
@@ -2561,7 +2576,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J34" s="67" t="n">
+      <c r="J34" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K34" s="2" t="n"/>
@@ -2613,7 +2628,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J35" s="78" t="n">
+      <c r="J35" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K35" s="2" t="n"/>
@@ -2665,7 +2680,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J36" s="78" t="n">
+      <c r="J36" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K36" s="2" t="n"/>
@@ -2717,7 +2732,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J37" s="78" t="n">
+      <c r="J37" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K37" s="2" t="n"/>
@@ -2769,7 +2784,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J38" s="78" t="n">
+      <c r="J38" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K38" s="2" t="n"/>
@@ -2821,7 +2836,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J39" s="78" t="n">
+      <c r="J39" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K39" s="2" t="n"/>
@@ -2873,7 +2888,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J40" s="78" t="n">
+      <c r="J40" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K40" s="2" t="n"/>
@@ -2925,7 +2940,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J41" s="78" t="n">
+      <c r="J41" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K41" s="2" t="n"/>
@@ -2977,7 +2992,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J42" s="78" t="n">
+      <c r="J42" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K42" s="2" t="n"/>
@@ -3029,7 +3044,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J43" s="67" t="n">
+      <c r="J43" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K43" s="2" t="n"/>
@@ -3081,7 +3096,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J44" s="78" t="n">
+      <c r="J44" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K44" s="2" t="n"/>
@@ -3133,7 +3148,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J45" s="67" t="n">
+      <c r="J45" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K45" s="2" t="n"/>
@@ -3185,7 +3200,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J46" s="78" t="n">
+      <c r="J46" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K46" s="2" t="n"/>
@@ -3237,7 +3252,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J47" s="78" t="n">
+      <c r="J47" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K47" s="2" t="n"/>
@@ -3289,7 +3304,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J48" s="67" t="n">
+      <c r="J48" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K48" s="2" t="n"/>
@@ -3341,7 +3356,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J49" s="78" t="n">
+      <c r="J49" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K49" s="2" t="n"/>
@@ -3393,7 +3408,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J50" s="78" t="n">
+      <c r="J50" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K50" s="2" t="n"/>
@@ -3445,7 +3460,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J51" s="78" t="n">
+      <c r="J51" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K51" s="2" t="n"/>
@@ -3497,7 +3512,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J52" s="67" t="n">
+      <c r="J52" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K52" s="2" t="n"/>
@@ -3549,7 +3564,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J53" s="78" t="n">
+      <c r="J53" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K53" s="2" t="n"/>
@@ -3601,7 +3616,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J54" s="67" t="n">
+      <c r="J54" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K54" s="2" t="n"/>
@@ -3653,7 +3668,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J55" s="67" t="n">
+      <c r="J55" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K55" s="2" t="n"/>
@@ -3705,7 +3720,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J56" s="78" t="n">
+      <c r="J56" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K56" s="2" t="n"/>
@@ -3757,7 +3772,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J57" s="78" t="n">
+      <c r="J57" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K57" s="2" t="n"/>
@@ -3809,7 +3824,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J58" s="78" t="n">
+      <c r="J58" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K58" s="2" t="n"/>
@@ -3861,7 +3876,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J59" s="67" t="n">
+      <c r="J59" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K59" s="2" t="n"/>
@@ -3913,7 +3928,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J60" s="67" t="n">
+      <c r="J60" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K60" s="2" t="n"/>
@@ -3965,7 +3980,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J61" s="67" t="n">
+      <c r="J61" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K61" s="2" t="n"/>
@@ -4017,7 +4032,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J62" s="78" t="n">
+      <c r="J62" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K62" s="2" t="n"/>
@@ -4069,7 +4084,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J63" s="78" t="n">
+      <c r="J63" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K63" s="2" t="n"/>
@@ -4121,7 +4136,7 @@
           <t>4 - 0</t>
         </is>
       </c>
-      <c r="J64" s="78" t="n">
+      <c r="J64" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K64" s="2" t="n"/>
@@ -4173,7 +4188,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J65" s="78" t="n">
+      <c r="J65" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K65" s="2" t="n"/>
@@ -4225,7 +4240,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J66" s="67" t="n">
+      <c r="J66" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K66" s="2" t="n"/>
@@ -4277,7 +4292,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J67" s="78" t="n">
+      <c r="J67" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K67" s="2" t="n"/>
@@ -4329,7 +4344,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J68" s="78" t="n">
+      <c r="J68" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K68" s="2" t="n"/>
@@ -4381,7 +4396,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J69" s="78" t="n">
+      <c r="J69" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K69" s="2" t="n"/>
@@ -4433,7 +4448,7 @@
           <t>2 - 3</t>
         </is>
       </c>
-      <c r="J70" s="78" t="n">
+      <c r="J70" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K70" s="2" t="n"/>
@@ -4485,7 +4500,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J71" s="67" t="n">
+      <c r="J71" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K71" s="2" t="n"/>
@@ -4537,7 +4552,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J72" s="78" t="n">
+      <c r="J72" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K72" s="2" t="n"/>
@@ -4589,7 +4604,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J73" s="78" t="n">
+      <c r="J73" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K73" s="2" t="n"/>
@@ -4641,7 +4656,7 @@
           <t>1 - 4</t>
         </is>
       </c>
-      <c r="J74" s="78" t="n">
+      <c r="J74" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K74" s="2" t="n"/>
@@ -4693,7 +4708,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J75" s="78" t="n">
+      <c r="J75" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K75" s="2" t="n"/>
@@ -4745,7 +4760,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J76" s="78" t="n">
+      <c r="J76" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K76" s="2" t="n"/>
@@ -4797,7 +4812,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J77" s="67" t="n">
+      <c r="J77" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K77" s="2" t="n"/>
@@ -4849,7 +4864,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J78" s="67" t="n">
+      <c r="J78" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K78" s="2" t="n"/>
@@ -4901,7 +4916,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J79" s="78" t="n">
+      <c r="J79" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K79" s="2" t="n"/>
@@ -4953,7 +4968,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J80" s="67" t="n">
+      <c r="J80" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K80" s="2" t="n"/>
@@ -5005,7 +5020,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J81" s="78" t="n">
+      <c r="J81" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K81" s="2" t="n"/>
@@ -5057,7 +5072,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J82" s="78" t="n">
+      <c r="J82" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K82" s="2" t="n"/>
@@ -5109,7 +5124,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J83" s="67" t="n">
+      <c r="J83" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K83" s="2" t="n"/>
@@ -5161,7 +5176,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J84" s="67" t="n">
+      <c r="J84" s="82" t="n">
         <v>0</v>
       </c>
       <c r="K84" s="2" t="n"/>
@@ -5213,7 +5228,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J85" s="78" t="n">
+      <c r="J85" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K85" s="2" t="n"/>
@@ -5265,7 +5280,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J86" s="78" t="n">
+      <c r="J86" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K86" s="2" t="n"/>
@@ -5317,7 +5332,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J87" s="78" t="n">
+      <c r="J87" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K87" s="2" t="n"/>
@@ -5369,7 +5384,7 @@
           <t>1 - 3</t>
         </is>
       </c>
-      <c r="J88" s="78" t="n">
+      <c r="J88" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K88" s="2" t="n"/>
@@ -5421,7 +5436,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J89" s="78" t="n">
+      <c r="J89" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K89" s="2" t="n"/>
@@ -5473,7 +5488,7 @@
           <t>1 - 6</t>
         </is>
       </c>
-      <c r="J90" s="78" t="n">
+      <c r="J90" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K90" s="2" t="n"/>
@@ -5525,7 +5540,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J91" s="78" t="n">
+      <c r="J91" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K91" s="2" t="n"/>
@@ -5577,7 +5592,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J92" s="78" t="n">
+      <c r="J92" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K92" s="2" t="n"/>
@@ -5629,7 +5644,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J93" s="78" t="n">
+      <c r="J93" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K93" s="2" t="n"/>
@@ -5681,7 +5696,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J94" s="78" t="n">
+      <c r="J94" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K94" s="2" t="n"/>
@@ -5733,7 +5748,7 @@
           <t>1 - 3</t>
         </is>
       </c>
-      <c r="J95" s="78" t="n">
+      <c r="J95" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K95" s="2" t="n"/>
@@ -5785,7 +5800,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J96" s="78" t="n">
+      <c r="J96" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K96" s="2" t="n"/>
@@ -5837,7 +5852,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J97" s="78" t="n">
+      <c r="J97" s="83" t="n">
         <v>1</v>
       </c>
       <c r="K97" s="2" t="n"/>
@@ -5850,6 +5865,422 @@
       <c r="R97" s="2" t="n"/>
       <c r="S97" s="2" t="n"/>
       <c r="T97" s="2" t="n"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="inlineStr">
+        <is>
+          <t>05.04.2025</t>
+        </is>
+      </c>
+      <c r="B98" s="2" t="inlineStr">
+        <is>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="inlineStr">
+        <is>
+          <t>Hoffenheim</t>
+        </is>
+      </c>
+      <c r="D98" s="2" t="inlineStr">
+        <is>
+          <t>IX</t>
+        </is>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="F98" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G98" s="2" t="n">
+        <v>60.5</v>
+      </c>
+      <c r="H98" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="I98" s="2" t="inlineStr">
+        <is>
+          <t>3 - 1</t>
+        </is>
+      </c>
+      <c r="J98" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="K98" s="2" t="n"/>
+      <c r="L98" s="2" t="n"/>
+      <c r="M98" s="2" t="n"/>
+      <c r="N98" s="2" t="n"/>
+      <c r="O98" s="2" t="n"/>
+      <c r="P98" s="2" t="n"/>
+      <c r="Q98" s="2" t="n"/>
+      <c r="R98" s="2" t="n"/>
+      <c r="S98" s="2" t="n"/>
+      <c r="T98" s="2" t="n"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="inlineStr">
+        <is>
+          <t>05.04.2025</t>
+        </is>
+      </c>
+      <c r="B99" s="2" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="C99" s="2" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="D99" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E99" s="2" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="F99" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G99" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="H99" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="I99" s="2" t="inlineStr">
+        <is>
+          <t>1 - 2</t>
+        </is>
+      </c>
+      <c r="J99" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" s="2" t="n"/>
+      <c r="L99" s="2" t="n"/>
+      <c r="M99" s="2" t="n"/>
+      <c r="N99" s="2" t="n"/>
+      <c r="O99" s="2" t="n"/>
+      <c r="P99" s="2" t="n"/>
+      <c r="Q99" s="2" t="n"/>
+      <c r="R99" s="2" t="n"/>
+      <c r="S99" s="2" t="n"/>
+      <c r="T99" s="2" t="n"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>05.04.2025</t>
+        </is>
+      </c>
+      <c r="B100" s="2" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="inlineStr">
+        <is>
+          <t>Angers</t>
+        </is>
+      </c>
+      <c r="D100" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E100" s="2" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="F100" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G100" s="2" t="n">
+        <v>56.49999999999999</v>
+      </c>
+      <c r="H100" s="2" t="n">
+        <v>6.499999999999993</v>
+      </c>
+      <c r="I100" s="2" t="inlineStr">
+        <is>
+          <t>1 - 0</t>
+        </is>
+      </c>
+      <c r="J100" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="K100" s="2" t="n"/>
+      <c r="L100" s="2" t="n"/>
+      <c r="M100" s="2" t="n"/>
+      <c r="N100" s="2" t="n"/>
+      <c r="O100" s="2" t="n"/>
+      <c r="P100" s="2" t="n"/>
+      <c r="Q100" s="2" t="n"/>
+      <c r="R100" s="2" t="n"/>
+      <c r="S100" s="2" t="n"/>
+      <c r="T100" s="2" t="n"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="inlineStr">
+        <is>
+          <t>05.04.2025</t>
+        </is>
+      </c>
+      <c r="B101" s="2" t="inlineStr">
+        <is>
+          <t>Parma</t>
+        </is>
+      </c>
+      <c r="C101" s="2" t="inlineStr">
+        <is>
+          <t>Inter Milan</t>
+        </is>
+      </c>
+      <c r="D101" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E101" s="2" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="F101" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G101" s="2" t="n">
+        <v>55.50000000000001</v>
+      </c>
+      <c r="H101" s="2" t="n">
+        <v>5.500000000000007</v>
+      </c>
+      <c r="I101" s="2" t="inlineStr">
+        <is>
+          <t>2 - 2</t>
+        </is>
+      </c>
+      <c r="J101" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="K101" s="2" t="n"/>
+      <c r="L101" s="2" t="n"/>
+      <c r="M101" s="2" t="n"/>
+      <c r="N101" s="2" t="n"/>
+      <c r="O101" s="2" t="n"/>
+      <c r="P101" s="2" t="n"/>
+      <c r="Q101" s="2" t="n"/>
+      <c r="R101" s="2" t="n"/>
+      <c r="S101" s="2" t="n"/>
+      <c r="T101" s="2" t="n"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="inlineStr">
+        <is>
+          <t>05.04.2025</t>
+        </is>
+      </c>
+      <c r="B102" s="2" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="C102" s="2" t="inlineStr">
+        <is>
+          <t>Betis</t>
+        </is>
+      </c>
+      <c r="D102" s="2" t="inlineStr">
+        <is>
+          <t>1X</t>
+        </is>
+      </c>
+      <c r="E102" s="2" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="F102" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G102" s="2" t="n">
+        <v>55.00000000000001</v>
+      </c>
+      <c r="H102" s="2" t="n">
+        <v>5.000000000000007</v>
+      </c>
+      <c r="I102" s="2" t="inlineStr">
+        <is>
+          <t>1 - 1</t>
+        </is>
+      </c>
+      <c r="J102" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="K102" s="2" t="n"/>
+      <c r="L102" s="2" t="n"/>
+      <c r="M102" s="2" t="n"/>
+      <c r="N102" s="2" t="n"/>
+      <c r="O102" s="2" t="n"/>
+      <c r="P102" s="2" t="n"/>
+      <c r="Q102" s="2" t="n"/>
+      <c r="R102" s="2" t="n"/>
+      <c r="S102" s="2" t="n"/>
+      <c r="T102" s="2" t="n"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="inlineStr">
+        <is>
+          <t>06.04.2025</t>
+        </is>
+      </c>
+      <c r="B103" s="2" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="C103" s="2" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="D103" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E103" s="2" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F103" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G103" s="2" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="H103" s="2" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I103" s="2" t="inlineStr">
+        <is>
+          <t>3 - 2</t>
+        </is>
+      </c>
+      <c r="J103" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="K103" s="2" t="n"/>
+      <c r="L103" s="2" t="n"/>
+      <c r="M103" s="2" t="n"/>
+      <c r="N103" s="2" t="n"/>
+      <c r="O103" s="2" t="n"/>
+      <c r="P103" s="2" t="n"/>
+      <c r="Q103" s="2" t="n"/>
+      <c r="R103" s="2" t="n"/>
+      <c r="S103" s="2" t="n"/>
+      <c r="T103" s="2" t="n"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="inlineStr">
+        <is>
+          <t>12.04.2025</t>
+        </is>
+      </c>
+      <c r="B104" s="2" t="inlineStr">
+        <is>
+          <t>Manchester City</t>
+        </is>
+      </c>
+      <c r="C104" s="2" t="inlineStr">
+        <is>
+          <t>Crystal Palace</t>
+        </is>
+      </c>
+      <c r="D104" s="2" t="inlineStr">
+        <is>
+          <t>1X</t>
+        </is>
+      </c>
+      <c r="E104" s="2" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="F104" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G104" s="2" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="H104" s="2" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="I104" s="2" t="inlineStr">
+        <is>
+          <t>5 - 2</t>
+        </is>
+      </c>
+      <c r="J104" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="K104" s="2" t="n"/>
+      <c r="L104" s="2" t="n"/>
+      <c r="M104" s="2" t="n"/>
+      <c r="N104" s="2" t="n"/>
+      <c r="O104" s="2" t="n"/>
+      <c r="P104" s="2" t="n"/>
+      <c r="Q104" s="2" t="n"/>
+      <c r="R104" s="2" t="n"/>
+      <c r="S104" s="2" t="n"/>
+      <c r="T104" s="2" t="n"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="inlineStr">
+        <is>
+          <t>12.04.2025</t>
+        </is>
+      </c>
+      <c r="B105" s="2" t="inlineStr">
+        <is>
+          <t>Bayer Leverkusen</t>
+        </is>
+      </c>
+      <c r="C105" s="2" t="inlineStr">
+        <is>
+          <t>Union Berlin</t>
+        </is>
+      </c>
+      <c r="D105" s="2" t="inlineStr">
+        <is>
+          <t>IX</t>
+        </is>
+      </c>
+      <c r="E105" s="2" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="F105" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G105" s="2" t="n">
+        <v>54.50000000000001</v>
+      </c>
+      <c r="H105" s="2" t="n">
+        <v>4.500000000000007</v>
+      </c>
+      <c r="I105" s="2" t="inlineStr">
+        <is>
+          <t>0 - 0</t>
+        </is>
+      </c>
+      <c r="J105" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="K105" s="2" t="n"/>
+      <c r="L105" s="2" t="n"/>
+      <c r="M105" s="2" t="n"/>
+      <c r="N105" s="2" t="n"/>
+      <c r="O105" s="2" t="n"/>
+      <c r="P105" s="2" t="n"/>
+      <c r="Q105" s="2" t="n"/>
+      <c r="R105" s="2" t="n"/>
+      <c r="S105" s="2" t="n"/>
+      <c r="T105" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5941,14 +6372,14 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>80.0%</t>
         </is>
       </c>
     </row>
@@ -5959,14 +6390,14 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>66.67%</t>
         </is>
       </c>
     </row>
@@ -6013,14 +6444,14 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>75.0%</t>
+          <t>60.0%</t>
         </is>
       </c>
     </row>
@@ -6031,14 +6462,14 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>77.78%</t>
+          <t>70.0%</t>
         </is>
       </c>
     </row>
@@ -6049,14 +6480,14 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>66.67%</t>
+          <t>71.43%</t>
         </is>
       </c>
     </row>
@@ -6139,14 +6570,14 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>1</v>
-      </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>66.67%</t>
         </is>
       </c>
     </row>
@@ -6193,10 +6624,10 @@
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
@@ -6373,14 +6804,14 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C28" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="C28" s="2" t="n">
-        <v>6</v>
-      </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>85.71%</t>
+          <t>87.5%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
manually add Man City and PSG on 10.05.2025
</commit_message>
<xml_diff>
--- a/app/placed_bets.xlsx
+++ b/app/placed_bets.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -377,6 +377,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -744,7 +762,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T121"/>
+  <dimension ref="A1:T129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -826,12 +844,12 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
-      <c r="L1" s="88" t="inlineStr">
+      <c r="L1" s="95" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="M1" s="86" t="inlineStr">
+      <c r="M1" s="93" t="inlineStr">
         <is>
           <t>Losses</t>
         </is>
@@ -910,27 +928,27 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J2" s="88" t="n">
+      <c r="J2" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>75</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>9020</v>
+        <v>9420</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>8311</v>
+        <v>8713.5</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>-709</v>
+        <v>-706.5</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
@@ -938,10 +956,10 @@
         </is>
       </c>
       <c r="S2" s="2" t="n">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>291</v>
+        <v>293.5</v>
       </c>
     </row>
     <row r="3">
@@ -982,7 +1000,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J3" s="86" t="n">
+      <c r="J3" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="n"/>
@@ -1034,7 +1052,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J4" s="88" t="n">
+      <c r="J4" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="n"/>
@@ -1086,7 +1104,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J5" s="88" t="n">
+      <c r="J5" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n"/>
@@ -1138,7 +1156,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J6" s="88" t="n">
+      <c r="J6" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="n"/>
@@ -1190,7 +1208,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J7" s="86" t="n">
+      <c r="J7" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="2" t="n"/>
@@ -1242,7 +1260,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J8" s="88" t="n">
+      <c r="J8" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="n"/>
@@ -1294,7 +1312,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J9" s="86" t="n">
+      <c r="J9" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="2" t="n"/>
@@ -1346,7 +1364,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J10" s="88" t="n">
+      <c r="J10" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K10" s="2" t="n"/>
@@ -1398,7 +1416,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J11" s="88" t="n">
+      <c r="J11" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K11" s="2" t="n"/>
@@ -1450,7 +1468,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J12" s="86" t="n">
+      <c r="J12" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="2" t="n"/>
@@ -1502,7 +1520,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J13" s="88" t="n">
+      <c r="J13" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K13" s="2" t="n"/>
@@ -1554,7 +1572,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J14" s="88" t="n">
+      <c r="J14" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="2" t="n"/>
@@ -1606,7 +1624,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J15" s="88" t="n">
+      <c r="J15" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K15" s="2" t="n"/>
@@ -1658,7 +1676,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J16" s="88" t="n">
+      <c r="J16" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K16" s="2" t="n"/>
@@ -1710,7 +1728,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J17" s="86" t="n">
+      <c r="J17" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K17" s="2" t="n"/>
@@ -1762,7 +1780,7 @@
           <t>5 - 0</t>
         </is>
       </c>
-      <c r="J18" s="88" t="n">
+      <c r="J18" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K18" s="2" t="n"/>
@@ -1814,7 +1832,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J19" s="86" t="n">
+      <c r="J19" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="2" t="n"/>
@@ -1866,7 +1884,7 @@
           <t>3 - 3</t>
         </is>
       </c>
-      <c r="J20" s="88" t="n">
+      <c r="J20" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K20" s="2" t="n"/>
@@ -1918,7 +1936,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J21" s="86" t="n">
+      <c r="J21" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K21" s="2" t="n"/>
@@ -1970,7 +1988,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J22" s="88" t="n">
+      <c r="J22" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K22" s="2" t="n"/>
@@ -2022,7 +2040,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J23" s="86" t="n">
+      <c r="J23" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K23" s="2" t="n"/>
@@ -2074,7 +2092,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J24" s="88" t="n">
+      <c r="J24" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K24" s="2" t="n"/>
@@ -2126,7 +2144,7 @@
           <t>0 - 6</t>
         </is>
       </c>
-      <c r="J25" s="88" t="n">
+      <c r="J25" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K25" s="2" t="n"/>
@@ -2178,7 +2196,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J26" s="88" t="n">
+      <c r="J26" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K26" s="2" t="n"/>
@@ -2230,7 +2248,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J27" s="88" t="n">
+      <c r="J27" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K27" s="2" t="n"/>
@@ -2282,7 +2300,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J28" s="88" t="n">
+      <c r="J28" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K28" s="2" t="n"/>
@@ -2334,7 +2352,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J29" s="86" t="n">
+      <c r="J29" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K29" s="2" t="n"/>
@@ -2386,7 +2404,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J30" s="88" t="n">
+      <c r="J30" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K30" s="2" t="n"/>
@@ -2438,7 +2456,7 @@
           <t>0 - 4</t>
         </is>
       </c>
-      <c r="J31" s="88" t="n">
+      <c r="J31" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K31" s="2" t="n"/>
@@ -2490,7 +2508,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J32" s="88" t="n">
+      <c r="J32" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K32" s="2" t="n"/>
@@ -2542,7 +2560,7 @@
           <t>2 - 5</t>
         </is>
       </c>
-      <c r="J33" s="88" t="n">
+      <c r="J33" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K33" s="2" t="n"/>
@@ -2594,7 +2612,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J34" s="86" t="n">
+      <c r="J34" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K34" s="2" t="n"/>
@@ -2646,7 +2664,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J35" s="88" t="n">
+      <c r="J35" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K35" s="2" t="n"/>
@@ -2698,7 +2716,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J36" s="88" t="n">
+      <c r="J36" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K36" s="2" t="n"/>
@@ -2750,7 +2768,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J37" s="88" t="n">
+      <c r="J37" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K37" s="2" t="n"/>
@@ -2802,7 +2820,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J38" s="88" t="n">
+      <c r="J38" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K38" s="2" t="n"/>
@@ -2854,7 +2872,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J39" s="88" t="n">
+      <c r="J39" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K39" s="2" t="n"/>
@@ -2906,7 +2924,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J40" s="88" t="n">
+      <c r="J40" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K40" s="2" t="n"/>
@@ -2958,7 +2976,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J41" s="88" t="n">
+      <c r="J41" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K41" s="2" t="n"/>
@@ -3010,7 +3028,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J42" s="88" t="n">
+      <c r="J42" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K42" s="2" t="n"/>
@@ -3062,7 +3080,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J43" s="86" t="n">
+      <c r="J43" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K43" s="2" t="n"/>
@@ -3114,7 +3132,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J44" s="88" t="n">
+      <c r="J44" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K44" s="2" t="n"/>
@@ -3166,7 +3184,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J45" s="86" t="n">
+      <c r="J45" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K45" s="2" t="n"/>
@@ -3218,7 +3236,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J46" s="88" t="n">
+      <c r="J46" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K46" s="2" t="n"/>
@@ -3270,7 +3288,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J47" s="88" t="n">
+      <c r="J47" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K47" s="2" t="n"/>
@@ -3322,7 +3340,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J48" s="86" t="n">
+      <c r="J48" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K48" s="2" t="n"/>
@@ -3374,7 +3392,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J49" s="88" t="n">
+      <c r="J49" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K49" s="2" t="n"/>
@@ -3426,7 +3444,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J50" s="88" t="n">
+      <c r="J50" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K50" s="2" t="n"/>
@@ -3478,7 +3496,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J51" s="88" t="n">
+      <c r="J51" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K51" s="2" t="n"/>
@@ -3530,7 +3548,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J52" s="86" t="n">
+      <c r="J52" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K52" s="2" t="n"/>
@@ -3582,7 +3600,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J53" s="88" t="n">
+      <c r="J53" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K53" s="2" t="n"/>
@@ -3634,7 +3652,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J54" s="86" t="n">
+      <c r="J54" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K54" s="2" t="n"/>
@@ -3686,7 +3704,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J55" s="86" t="n">
+      <c r="J55" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K55" s="2" t="n"/>
@@ -3738,7 +3756,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J56" s="88" t="n">
+      <c r="J56" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K56" s="2" t="n"/>
@@ -3790,7 +3808,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J57" s="88" t="n">
+      <c r="J57" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K57" s="2" t="n"/>
@@ -3842,7 +3860,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J58" s="88" t="n">
+      <c r="J58" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K58" s="2" t="n"/>
@@ -3894,7 +3912,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J59" s="86" t="n">
+      <c r="J59" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K59" s="2" t="n"/>
@@ -3946,7 +3964,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J60" s="86" t="n">
+      <c r="J60" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K60" s="2" t="n"/>
@@ -3998,7 +4016,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J61" s="86" t="n">
+      <c r="J61" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K61" s="2" t="n"/>
@@ -4050,7 +4068,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J62" s="88" t="n">
+      <c r="J62" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K62" s="2" t="n"/>
@@ -4102,7 +4120,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J63" s="88" t="n">
+      <c r="J63" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K63" s="2" t="n"/>
@@ -4154,7 +4172,7 @@
           <t>4 - 0</t>
         </is>
       </c>
-      <c r="J64" s="88" t="n">
+      <c r="J64" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K64" s="2" t="n"/>
@@ -4206,7 +4224,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J65" s="88" t="n">
+      <c r="J65" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K65" s="2" t="n"/>
@@ -4258,7 +4276,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J66" s="86" t="n">
+      <c r="J66" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K66" s="2" t="n"/>
@@ -4310,7 +4328,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J67" s="88" t="n">
+      <c r="J67" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K67" s="2" t="n"/>
@@ -4362,7 +4380,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J68" s="88" t="n">
+      <c r="J68" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K68" s="2" t="n"/>
@@ -4414,7 +4432,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J69" s="88" t="n">
+      <c r="J69" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K69" s="2" t="n"/>
@@ -4466,7 +4484,7 @@
           <t>2 - 3</t>
         </is>
       </c>
-      <c r="J70" s="88" t="n">
+      <c r="J70" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K70" s="2" t="n"/>
@@ -4518,7 +4536,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J71" s="86" t="n">
+      <c r="J71" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K71" s="2" t="n"/>
@@ -4570,7 +4588,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J72" s="88" t="n">
+      <c r="J72" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K72" s="2" t="n"/>
@@ -4622,7 +4640,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J73" s="88" t="n">
+      <c r="J73" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K73" s="2" t="n"/>
@@ -4674,7 +4692,7 @@
           <t>1 - 4</t>
         </is>
       </c>
-      <c r="J74" s="88" t="n">
+      <c r="J74" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K74" s="2" t="n"/>
@@ -4726,7 +4744,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J75" s="88" t="n">
+      <c r="J75" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K75" s="2" t="n"/>
@@ -4778,7 +4796,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J76" s="88" t="n">
+      <c r="J76" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K76" s="2" t="n"/>
@@ -4830,7 +4848,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J77" s="86" t="n">
+      <c r="J77" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K77" s="2" t="n"/>
@@ -4882,7 +4900,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J78" s="86" t="n">
+      <c r="J78" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K78" s="2" t="n"/>
@@ -4934,7 +4952,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J79" s="88" t="n">
+      <c r="J79" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K79" s="2" t="n"/>
@@ -4986,7 +5004,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J80" s="86" t="n">
+      <c r="J80" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K80" s="2" t="n"/>
@@ -5038,7 +5056,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J81" s="88" t="n">
+      <c r="J81" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K81" s="2" t="n"/>
@@ -5090,7 +5108,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J82" s="88" t="n">
+      <c r="J82" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K82" s="2" t="n"/>
@@ -5142,7 +5160,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J83" s="86" t="n">
+      <c r="J83" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K83" s="2" t="n"/>
@@ -5194,7 +5212,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J84" s="86" t="n">
+      <c r="J84" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K84" s="2" t="n"/>
@@ -5246,7 +5264,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J85" s="88" t="n">
+      <c r="J85" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K85" s="2" t="n"/>
@@ -5298,7 +5316,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J86" s="88" t="n">
+      <c r="J86" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K86" s="2" t="n"/>
@@ -5350,7 +5368,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J87" s="88" t="n">
+      <c r="J87" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K87" s="2" t="n"/>
@@ -5402,7 +5420,7 @@
           <t>1 - 3</t>
         </is>
       </c>
-      <c r="J88" s="88" t="n">
+      <c r="J88" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K88" s="2" t="n"/>
@@ -5454,7 +5472,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J89" s="88" t="n">
+      <c r="J89" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K89" s="2" t="n"/>
@@ -5506,7 +5524,7 @@
           <t>1 - 6</t>
         </is>
       </c>
-      <c r="J90" s="88" t="n">
+      <c r="J90" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K90" s="2" t="n"/>
@@ -5558,7 +5576,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J91" s="88" t="n">
+      <c r="J91" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K91" s="2" t="n"/>
@@ -5610,7 +5628,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J92" s="88" t="n">
+      <c r="J92" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K92" s="2" t="n"/>
@@ -5662,7 +5680,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J93" s="88" t="n">
+      <c r="J93" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K93" s="2" t="n"/>
@@ -5714,7 +5732,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J94" s="88" t="n">
+      <c r="J94" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K94" s="2" t="n"/>
@@ -5766,7 +5784,7 @@
           <t>1 - 3</t>
         </is>
       </c>
-      <c r="J95" s="88" t="n">
+      <c r="J95" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K95" s="2" t="n"/>
@@ -5818,7 +5836,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J96" s="88" t="n">
+      <c r="J96" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K96" s="2" t="n"/>
@@ -5870,7 +5888,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J97" s="88" t="n">
+      <c r="J97" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K97" s="2" t="n"/>
@@ -5922,7 +5940,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J98" s="88" t="n">
+      <c r="J98" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K98" s="2" t="n"/>
@@ -5974,7 +5992,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J99" s="86" t="n">
+      <c r="J99" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K99" s="2" t="n"/>
@@ -6026,7 +6044,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J100" s="88" t="n">
+      <c r="J100" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K100" s="2" t="n"/>
@@ -6078,7 +6096,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J101" s="88" t="n">
+      <c r="J101" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K101" s="2" t="n"/>
@@ -6130,7 +6148,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J102" s="88" t="n">
+      <c r="J102" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K102" s="2" t="n"/>
@@ -6182,7 +6200,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J103" s="86" t="n">
+      <c r="J103" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K103" s="2" t="n"/>
@@ -6234,7 +6252,7 @@
           <t>5 - 2</t>
         </is>
       </c>
-      <c r="J104" s="88" t="n">
+      <c r="J104" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K104" s="2" t="n"/>
@@ -6286,7 +6304,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J105" s="88" t="n">
+      <c r="J105" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K105" s="2" t="n"/>
@@ -6338,7 +6356,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J106" s="88" t="n">
+      <c r="J106" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K106" s="2" t="n"/>
@@ -6390,7 +6408,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J107" s="88" t="n">
+      <c r="J107" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K107" s="2" t="n"/>
@@ -6442,7 +6460,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J108" s="88" t="n">
+      <c r="J108" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K108" s="2" t="n"/>
@@ -6494,7 +6512,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J109" s="86" t="n">
+      <c r="J109" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K109" s="2" t="n"/>
@@ -6546,7 +6564,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J110" s="88" t="n">
+      <c r="J110" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K110" s="2" t="n"/>
@@ -6598,7 +6616,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J111" s="88" t="n">
+      <c r="J111" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K111" s="2" t="n"/>
@@ -6650,7 +6668,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J112" s="88" t="n">
+      <c r="J112" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K112" s="2" t="n"/>
@@ -6702,7 +6720,7 @@
           <t>0 - 4</t>
         </is>
       </c>
-      <c r="J113" s="88" t="n">
+      <c r="J113" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K113" s="2" t="n"/>
@@ -6754,7 +6772,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J114" s="88" t="n">
+      <c r="J114" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K114" s="2" t="n"/>
@@ -6806,7 +6824,7 @@
           <t>4 - 3</t>
         </is>
       </c>
-      <c r="J115" s="88" t="n">
+      <c r="J115" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K115" s="2" t="n"/>
@@ -6858,7 +6876,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J116" s="88" t="n">
+      <c r="J116" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K116" s="2" t="n"/>
@@ -6910,7 +6928,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J117" s="88" t="n">
+      <c r="J117" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K117" s="2" t="n"/>
@@ -6962,7 +6980,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J118" s="88" t="n">
+      <c r="J118" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K118" s="2" t="n"/>
@@ -7014,7 +7032,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J119" s="86" t="n">
+      <c r="J119" s="93" t="n">
         <v>0</v>
       </c>
       <c r="K119" s="2" t="n"/>
@@ -7066,7 +7084,7 @@
           <t>0 - 4</t>
         </is>
       </c>
-      <c r="J120" s="88" t="n">
+      <c r="J120" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K120" s="2" t="n"/>
@@ -7118,7 +7136,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J121" s="88" t="n">
+      <c r="J121" s="95" t="n">
         <v>1</v>
       </c>
       <c r="K121" s="2" t="n"/>
@@ -7131,6 +7149,422 @@
       <c r="R121" s="2" t="n"/>
       <c r="S121" s="2" t="n"/>
       <c r="T121" s="2" t="n"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="inlineStr">
+        <is>
+          <t>20.04.2025</t>
+        </is>
+      </c>
+      <c r="B122" s="2" t="inlineStr">
+        <is>
+          <t>Saint Etienne</t>
+        </is>
+      </c>
+      <c r="C122" s="2" t="inlineStr">
+        <is>
+          <t>Olympique Lyon</t>
+        </is>
+      </c>
+      <c r="D122" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E122" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F122" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G122" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="H122" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I122" s="2" t="inlineStr">
+        <is>
+          <t>2 - 1</t>
+        </is>
+      </c>
+      <c r="J122" s="93" t="n">
+        <v>0</v>
+      </c>
+      <c r="K122" s="2" t="n"/>
+      <c r="L122" s="2" t="n"/>
+      <c r="M122" s="2" t="n"/>
+      <c r="N122" s="2" t="n"/>
+      <c r="O122" s="2" t="n"/>
+      <c r="P122" s="2" t="n"/>
+      <c r="Q122" s="2" t="n"/>
+      <c r="R122" s="2" t="n"/>
+      <c r="S122" s="2" t="n"/>
+      <c r="T122" s="2" t="n"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="inlineStr">
+        <is>
+          <t>22.04.2025</t>
+        </is>
+      </c>
+      <c r="B123" s="2" t="inlineStr">
+        <is>
+          <t>Nantes</t>
+        </is>
+      </c>
+      <c r="C123" s="2" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="D123" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E123" s="2" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="F123" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G123" s="2" t="n">
+        <v>56.00000000000001</v>
+      </c>
+      <c r="H123" s="2" t="n">
+        <v>6.000000000000007</v>
+      </c>
+      <c r="I123" s="2" t="inlineStr">
+        <is>
+          <t>1 - 1</t>
+        </is>
+      </c>
+      <c r="J123" s="95" t="n">
+        <v>1</v>
+      </c>
+      <c r="K123" s="2" t="n"/>
+      <c r="L123" s="2" t="n"/>
+      <c r="M123" s="2" t="n"/>
+      <c r="N123" s="2" t="n"/>
+      <c r="O123" s="2" t="n"/>
+      <c r="P123" s="2" t="n"/>
+      <c r="Q123" s="2" t="n"/>
+      <c r="R123" s="2" t="n"/>
+      <c r="S123" s="2" t="n"/>
+      <c r="T123" s="2" t="n"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="inlineStr">
+        <is>
+          <t>22.04.2025</t>
+        </is>
+      </c>
+      <c r="B124" s="2" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="C124" s="2" t="inlineStr">
+        <is>
+          <t>Mallorca</t>
+        </is>
+      </c>
+      <c r="D124" s="2" t="inlineStr">
+        <is>
+          <t>IX</t>
+        </is>
+      </c>
+      <c r="E124" s="2" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="F124" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G124" s="2" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="H124" s="2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="I124" s="2" t="inlineStr">
+        <is>
+          <t>1 - 0</t>
+        </is>
+      </c>
+      <c r="J124" s="95" t="n">
+        <v>1</v>
+      </c>
+      <c r="K124" s="2" t="n"/>
+      <c r="L124" s="2" t="n"/>
+      <c r="M124" s="2" t="n"/>
+      <c r="N124" s="2" t="n"/>
+      <c r="O124" s="2" t="n"/>
+      <c r="P124" s="2" t="n"/>
+      <c r="Q124" s="2" t="n"/>
+      <c r="R124" s="2" t="n"/>
+      <c r="S124" s="2" t="n"/>
+      <c r="T124" s="2" t="n"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="inlineStr">
+        <is>
+          <t>23.04.2025</t>
+        </is>
+      </c>
+      <c r="B125" s="2" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="C125" s="2" t="inlineStr">
+        <is>
+          <t>Crystal Palace</t>
+        </is>
+      </c>
+      <c r="D125" s="2" t="inlineStr">
+        <is>
+          <t>IX</t>
+        </is>
+      </c>
+      <c r="E125" s="2" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="F125" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G125" s="2" t="n">
+        <v>54.50000000000001</v>
+      </c>
+      <c r="H125" s="2" t="n">
+        <v>4.500000000000007</v>
+      </c>
+      <c r="I125" s="2" t="inlineStr">
+        <is>
+          <t>2 - 2</t>
+        </is>
+      </c>
+      <c r="J125" s="95" t="n">
+        <v>1</v>
+      </c>
+      <c r="K125" s="2" t="n"/>
+      <c r="L125" s="2" t="n"/>
+      <c r="M125" s="2" t="n"/>
+      <c r="N125" s="2" t="n"/>
+      <c r="O125" s="2" t="n"/>
+      <c r="P125" s="2" t="n"/>
+      <c r="Q125" s="2" t="n"/>
+      <c r="R125" s="2" t="n"/>
+      <c r="S125" s="2" t="n"/>
+      <c r="T125" s="2" t="n"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="inlineStr">
+        <is>
+          <t>10.05.2025</t>
+        </is>
+      </c>
+      <c r="B126" s="2" t="inlineStr">
+        <is>
+          <t>Southampton</t>
+        </is>
+      </c>
+      <c r="C126" s="2" t="inlineStr">
+        <is>
+          <t>Manchester City</t>
+        </is>
+      </c>
+      <c r="D126" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E126" s="2" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="F126" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G126" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="H126" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="I126" s="2" t="inlineStr">
+        <is>
+          <t>0 - 0</t>
+        </is>
+      </c>
+      <c r="J126" s="93" t="n">
+        <v>0</v>
+      </c>
+      <c r="K126" s="2" t="n"/>
+      <c r="L126" s="2" t="n"/>
+      <c r="M126" s="2" t="n"/>
+      <c r="N126" s="2" t="n"/>
+      <c r="O126" s="2" t="n"/>
+      <c r="P126" s="2" t="n"/>
+      <c r="Q126" s="2" t="n"/>
+      <c r="R126" s="2" t="n"/>
+      <c r="S126" s="2" t="n"/>
+      <c r="T126" s="2" t="n"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="inlineStr">
+        <is>
+          <t>10.05.2025</t>
+        </is>
+      </c>
+      <c r="B127" s="2" t="inlineStr">
+        <is>
+          <t>Le Havre</t>
+        </is>
+      </c>
+      <c r="C127" s="2" t="inlineStr">
+        <is>
+          <t>Olympique Marseille</t>
+        </is>
+      </c>
+      <c r="D127" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E127" s="2" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="F127" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G127" s="2" t="n">
+        <v>73.5</v>
+      </c>
+      <c r="H127" s="2" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="I127" s="2" t="inlineStr">
+        <is>
+          <t>1 - 3</t>
+        </is>
+      </c>
+      <c r="J127" s="95" t="n">
+        <v>1</v>
+      </c>
+      <c r="K127" s="2" t="n"/>
+      <c r="L127" s="2" t="n"/>
+      <c r="M127" s="2" t="n"/>
+      <c r="N127" s="2" t="n"/>
+      <c r="O127" s="2" t="n"/>
+      <c r="P127" s="2" t="n"/>
+      <c r="Q127" s="2" t="n"/>
+      <c r="R127" s="2" t="n"/>
+      <c r="S127" s="2" t="n"/>
+      <c r="T127" s="2" t="n"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="inlineStr">
+        <is>
+          <t>10.05.2025</t>
+        </is>
+      </c>
+      <c r="B128" s="2" t="inlineStr">
+        <is>
+          <t>Montpellier</t>
+        </is>
+      </c>
+      <c r="C128" s="2" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="D128" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E128" s="2" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="F128" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G128" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="H128" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="I128" s="2" t="inlineStr">
+        <is>
+          <t>1 - 4</t>
+        </is>
+      </c>
+      <c r="J128" s="95" t="n">
+        <v>1</v>
+      </c>
+      <c r="K128" s="2" t="n"/>
+      <c r="L128" s="2" t="n"/>
+      <c r="M128" s="2" t="n"/>
+      <c r="N128" s="2" t="n"/>
+      <c r="O128" s="2" t="n"/>
+      <c r="P128" s="2" t="n"/>
+      <c r="Q128" s="2" t="n"/>
+      <c r="R128" s="2" t="n"/>
+      <c r="S128" s="2" t="n"/>
+      <c r="T128" s="2" t="n"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="inlineStr">
+        <is>
+          <t>10.05.2025</t>
+        </is>
+      </c>
+      <c r="B129" s="2" t="inlineStr">
+        <is>
+          <t>Atletico Madrid</t>
+        </is>
+      </c>
+      <c r="C129" s="2" t="inlineStr">
+        <is>
+          <t>Real Sociedad</t>
+        </is>
+      </c>
+      <c r="D129" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E129" s="2" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="F129" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G129" s="2" t="n">
+        <v>94</v>
+      </c>
+      <c r="H129" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="I129" s="2" t="inlineStr">
+        <is>
+          <t>4 - 0</t>
+        </is>
+      </c>
+      <c r="J129" s="95" t="n">
+        <v>1</v>
+      </c>
+      <c r="K129" s="2" t="n"/>
+      <c r="L129" s="2" t="n"/>
+      <c r="M129" s="2" t="n"/>
+      <c r="N129" s="2" t="n"/>
+      <c r="O129" s="2" t="n"/>
+      <c r="P129" s="2" t="n"/>
+      <c r="Q129" s="2" t="n"/>
+      <c r="R129" s="2" t="n"/>
+      <c r="S129" s="2" t="n"/>
+      <c r="T129" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7186,14 +7620,14 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>60.0%</t>
+          <t>66.67%</t>
         </is>
       </c>
     </row>
@@ -7240,14 +7674,14 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>66.67%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -7276,14 +7710,14 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>42.86%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -7294,14 +7728,14 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>57.14%</t>
+          <t>62.5%</t>
         </is>
       </c>
     </row>
@@ -7582,14 +8016,14 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>33.33%</t>
         </is>
       </c>
     </row>
@@ -7600,14 +8034,14 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>60.0%</t>
+          <t>66.67%</t>
         </is>
       </c>
     </row>
@@ -7654,14 +8088,14 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>88.89%</t>
+          <t>90.91%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update GW6 2025/26 - scrap containerization
</commit_message>
<xml_diff>
--- a/app/placed_bets.xlsx
+++ b/app/placed_bets.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -434,6 +434,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -807,7 +822,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T159"/>
+  <dimension ref="A1:T164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -889,12 +904,12 @@
         </is>
       </c>
       <c r="K1" s="2" t="n"/>
-      <c r="L1" s="110" t="inlineStr">
+      <c r="L1" s="115" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="M1" s="108" t="inlineStr">
+      <c r="M1" s="114" t="inlineStr">
         <is>
           <t>Losses</t>
         </is>
@@ -973,38 +988,38 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J2" s="110" t="n">
+      <c r="J2" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>74.68000000000001</v>
+        <v>74.23</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>10800</v>
+        <v>11010</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>10026.5</v>
+        <v>10220.5</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>-773.5</v>
+        <v>-789.5</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
-          <t>-0.75%</t>
+          <t>-0.76%</t>
         </is>
       </c>
       <c r="S2" s="2" t="n">
         <v>1.31</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>246.5</v>
+        <v>240.5</v>
       </c>
     </row>
     <row r="3">
@@ -1045,7 +1060,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J3" s="108" t="n">
+      <c r="J3" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="n"/>
@@ -1097,7 +1112,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J4" s="110" t="n">
+      <c r="J4" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="n"/>
@@ -1149,7 +1164,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J5" s="110" t="n">
+      <c r="J5" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n"/>
@@ -1201,7 +1216,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J6" s="110" t="n">
+      <c r="J6" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="n"/>
@@ -1253,7 +1268,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J7" s="108" t="n">
+      <c r="J7" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="2" t="n"/>
@@ -1305,7 +1320,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J8" s="110" t="n">
+      <c r="J8" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="n"/>
@@ -1357,7 +1372,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J9" s="108" t="n">
+      <c r="J9" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="2" t="n"/>
@@ -1409,7 +1424,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J10" s="110" t="n">
+      <c r="J10" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K10" s="2" t="n"/>
@@ -1461,7 +1476,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J11" s="110" t="n">
+      <c r="J11" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K11" s="2" t="n"/>
@@ -1513,7 +1528,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J12" s="108" t="n">
+      <c r="J12" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="2" t="n"/>
@@ -1565,7 +1580,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J13" s="110" t="n">
+      <c r="J13" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K13" s="2" t="n"/>
@@ -1617,7 +1632,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J14" s="110" t="n">
+      <c r="J14" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K14" s="2" t="n"/>
@@ -1669,7 +1684,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J15" s="110" t="n">
+      <c r="J15" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K15" s="2" t="n"/>
@@ -1721,7 +1736,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J16" s="110" t="n">
+      <c r="J16" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K16" s="2" t="n"/>
@@ -1773,7 +1788,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J17" s="108" t="n">
+      <c r="J17" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K17" s="2" t="n"/>
@@ -1825,7 +1840,7 @@
           <t>5 - 0</t>
         </is>
       </c>
-      <c r="J18" s="110" t="n">
+      <c r="J18" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K18" s="2" t="n"/>
@@ -1877,7 +1892,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J19" s="108" t="n">
+      <c r="J19" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="2" t="n"/>
@@ -1929,7 +1944,7 @@
           <t>3 - 3</t>
         </is>
       </c>
-      <c r="J20" s="110" t="n">
+      <c r="J20" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K20" s="2" t="n"/>
@@ -1981,7 +1996,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J21" s="108" t="n">
+      <c r="J21" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K21" s="2" t="n"/>
@@ -2033,7 +2048,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J22" s="110" t="n">
+      <c r="J22" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K22" s="2" t="n"/>
@@ -2085,7 +2100,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J23" s="108" t="n">
+      <c r="J23" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K23" s="2" t="n"/>
@@ -2137,7 +2152,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J24" s="110" t="n">
+      <c r="J24" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K24" s="2" t="n"/>
@@ -2189,7 +2204,7 @@
           <t>0 - 6</t>
         </is>
       </c>
-      <c r="J25" s="110" t="n">
+      <c r="J25" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K25" s="2" t="n"/>
@@ -2241,7 +2256,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J26" s="110" t="n">
+      <c r="J26" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K26" s="2" t="n"/>
@@ -2293,7 +2308,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J27" s="110" t="n">
+      <c r="J27" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K27" s="2" t="n"/>
@@ -2345,7 +2360,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J28" s="110" t="n">
+      <c r="J28" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K28" s="2" t="n"/>
@@ -2397,7 +2412,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J29" s="108" t="n">
+      <c r="J29" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K29" s="2" t="n"/>
@@ -2449,7 +2464,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J30" s="110" t="n">
+      <c r="J30" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K30" s="2" t="n"/>
@@ -2501,7 +2516,7 @@
           <t>0 - 4</t>
         </is>
       </c>
-      <c r="J31" s="110" t="n">
+      <c r="J31" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K31" s="2" t="n"/>
@@ -2553,7 +2568,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J32" s="110" t="n">
+      <c r="J32" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K32" s="2" t="n"/>
@@ -2605,7 +2620,7 @@
           <t>2 - 5</t>
         </is>
       </c>
-      <c r="J33" s="110" t="n">
+      <c r="J33" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K33" s="2" t="n"/>
@@ -2657,7 +2672,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J34" s="108" t="n">
+      <c r="J34" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K34" s="2" t="n"/>
@@ -2709,7 +2724,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J35" s="110" t="n">
+      <c r="J35" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K35" s="2" t="n"/>
@@ -2761,7 +2776,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J36" s="110" t="n">
+      <c r="J36" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K36" s="2" t="n"/>
@@ -2813,7 +2828,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J37" s="110" t="n">
+      <c r="J37" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K37" s="2" t="n"/>
@@ -2865,7 +2880,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J38" s="110" t="n">
+      <c r="J38" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K38" s="2" t="n"/>
@@ -2917,7 +2932,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J39" s="110" t="n">
+      <c r="J39" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K39" s="2" t="n"/>
@@ -2969,7 +2984,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J40" s="110" t="n">
+      <c r="J40" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K40" s="2" t="n"/>
@@ -3021,7 +3036,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J41" s="110" t="n">
+      <c r="J41" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K41" s="2" t="n"/>
@@ -3073,7 +3088,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J42" s="110" t="n">
+      <c r="J42" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K42" s="2" t="n"/>
@@ -3125,7 +3140,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J43" s="108" t="n">
+      <c r="J43" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K43" s="2" t="n"/>
@@ -3177,7 +3192,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J44" s="110" t="n">
+      <c r="J44" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K44" s="2" t="n"/>
@@ -3229,7 +3244,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J45" s="108" t="n">
+      <c r="J45" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K45" s="2" t="n"/>
@@ -3281,7 +3296,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J46" s="110" t="n">
+      <c r="J46" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K46" s="2" t="n"/>
@@ -3333,7 +3348,7 @@
           <t>5 - 1</t>
         </is>
       </c>
-      <c r="J47" s="110" t="n">
+      <c r="J47" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K47" s="2" t="n"/>
@@ -3385,7 +3400,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J48" s="108" t="n">
+      <c r="J48" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K48" s="2" t="n"/>
@@ -3437,7 +3452,7 @@
           <t>7 - 1</t>
         </is>
       </c>
-      <c r="J49" s="110" t="n">
+      <c r="J49" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K49" s="2" t="n"/>
@@ -3489,7 +3504,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J50" s="110" t="n">
+      <c r="J50" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K50" s="2" t="n"/>
@@ -3541,7 +3556,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J51" s="110" t="n">
+      <c r="J51" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K51" s="2" t="n"/>
@@ -3593,7 +3608,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J52" s="108" t="n">
+      <c r="J52" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K52" s="2" t="n"/>
@@ -3645,7 +3660,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J53" s="110" t="n">
+      <c r="J53" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K53" s="2" t="n"/>
@@ -3697,7 +3712,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J54" s="108" t="n">
+      <c r="J54" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K54" s="2" t="n"/>
@@ -3749,7 +3764,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J55" s="108" t="n">
+      <c r="J55" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K55" s="2" t="n"/>
@@ -3801,7 +3816,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J56" s="110" t="n">
+      <c r="J56" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K56" s="2" t="n"/>
@@ -3853,7 +3868,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J57" s="110" t="n">
+      <c r="J57" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K57" s="2" t="n"/>
@@ -3905,7 +3920,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J58" s="110" t="n">
+      <c r="J58" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K58" s="2" t="n"/>
@@ -3957,7 +3972,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J59" s="108" t="n">
+      <c r="J59" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K59" s="2" t="n"/>
@@ -4009,7 +4024,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J60" s="108" t="n">
+      <c r="J60" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K60" s="2" t="n"/>
@@ -4061,7 +4076,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J61" s="108" t="n">
+      <c r="J61" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K61" s="2" t="n"/>
@@ -4113,7 +4128,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J62" s="110" t="n">
+      <c r="J62" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K62" s="2" t="n"/>
@@ -4165,7 +4180,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J63" s="110" t="n">
+      <c r="J63" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K63" s="2" t="n"/>
@@ -4217,7 +4232,7 @@
           <t>4 - 0</t>
         </is>
       </c>
-      <c r="J64" s="110" t="n">
+      <c r="J64" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K64" s="2" t="n"/>
@@ -4269,7 +4284,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J65" s="110" t="n">
+      <c r="J65" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K65" s="2" t="n"/>
@@ -4321,7 +4336,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J66" s="108" t="n">
+      <c r="J66" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K66" s="2" t="n"/>
@@ -4373,7 +4388,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J67" s="110" t="n">
+      <c r="J67" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K67" s="2" t="n"/>
@@ -4425,7 +4440,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J68" s="110" t="n">
+      <c r="J68" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K68" s="2" t="n"/>
@@ -4477,7 +4492,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J69" s="110" t="n">
+      <c r="J69" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K69" s="2" t="n"/>
@@ -4529,7 +4544,7 @@
           <t>2 - 3</t>
         </is>
       </c>
-      <c r="J70" s="110" t="n">
+      <c r="J70" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K70" s="2" t="n"/>
@@ -4581,7 +4596,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J71" s="108" t="n">
+      <c r="J71" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K71" s="2" t="n"/>
@@ -4633,7 +4648,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J72" s="110" t="n">
+      <c r="J72" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K72" s="2" t="n"/>
@@ -4685,7 +4700,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J73" s="110" t="n">
+      <c r="J73" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K73" s="2" t="n"/>
@@ -4737,7 +4752,7 @@
           <t>1 - 4</t>
         </is>
       </c>
-      <c r="J74" s="110" t="n">
+      <c r="J74" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K74" s="2" t="n"/>
@@ -4789,7 +4804,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J75" s="110" t="n">
+      <c r="J75" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K75" s="2" t="n"/>
@@ -4841,7 +4856,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J76" s="110" t="n">
+      <c r="J76" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K76" s="2" t="n"/>
@@ -4893,7 +4908,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J77" s="108" t="n">
+      <c r="J77" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K77" s="2" t="n"/>
@@ -4945,7 +4960,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J78" s="108" t="n">
+      <c r="J78" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K78" s="2" t="n"/>
@@ -4997,7 +5012,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J79" s="110" t="n">
+      <c r="J79" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K79" s="2" t="n"/>
@@ -5049,7 +5064,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J80" s="108" t="n">
+      <c r="J80" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K80" s="2" t="n"/>
@@ -5101,7 +5116,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J81" s="110" t="n">
+      <c r="J81" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K81" s="2" t="n"/>
@@ -5153,7 +5168,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J82" s="110" t="n">
+      <c r="J82" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K82" s="2" t="n"/>
@@ -5205,7 +5220,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J83" s="108" t="n">
+      <c r="J83" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K83" s="2" t="n"/>
@@ -5257,7 +5272,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J84" s="108" t="n">
+      <c r="J84" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K84" s="2" t="n"/>
@@ -5309,7 +5324,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J85" s="110" t="n">
+      <c r="J85" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K85" s="2" t="n"/>
@@ -5361,7 +5376,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J86" s="110" t="n">
+      <c r="J86" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K86" s="2" t="n"/>
@@ -5413,7 +5428,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J87" s="110" t="n">
+      <c r="J87" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K87" s="2" t="n"/>
@@ -5465,7 +5480,7 @@
           <t>1 - 3</t>
         </is>
       </c>
-      <c r="J88" s="110" t="n">
+      <c r="J88" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K88" s="2" t="n"/>
@@ -5517,7 +5532,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J89" s="110" t="n">
+      <c r="J89" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K89" s="2" t="n"/>
@@ -5569,7 +5584,7 @@
           <t>1 - 6</t>
         </is>
       </c>
-      <c r="J90" s="110" t="n">
+      <c r="J90" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K90" s="2" t="n"/>
@@ -5621,7 +5636,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J91" s="110" t="n">
+      <c r="J91" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K91" s="2" t="n"/>
@@ -5673,7 +5688,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J92" s="110" t="n">
+      <c r="J92" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K92" s="2" t="n"/>
@@ -5725,7 +5740,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J93" s="110" t="n">
+      <c r="J93" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K93" s="2" t="n"/>
@@ -5777,7 +5792,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J94" s="110" t="n">
+      <c r="J94" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K94" s="2" t="n"/>
@@ -5829,7 +5844,7 @@
           <t>1 - 3</t>
         </is>
       </c>
-      <c r="J95" s="110" t="n">
+      <c r="J95" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K95" s="2" t="n"/>
@@ -5881,7 +5896,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J96" s="110" t="n">
+      <c r="J96" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K96" s="2" t="n"/>
@@ -5933,7 +5948,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J97" s="110" t="n">
+      <c r="J97" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K97" s="2" t="n"/>
@@ -5985,7 +6000,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J98" s="110" t="n">
+      <c r="J98" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K98" s="2" t="n"/>
@@ -6037,7 +6052,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J99" s="108" t="n">
+      <c r="J99" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K99" s="2" t="n"/>
@@ -6089,7 +6104,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J100" s="110" t="n">
+      <c r="J100" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K100" s="2" t="n"/>
@@ -6141,7 +6156,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J101" s="110" t="n">
+      <c r="J101" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K101" s="2" t="n"/>
@@ -6193,7 +6208,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J102" s="110" t="n">
+      <c r="J102" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K102" s="2" t="n"/>
@@ -6245,7 +6260,7 @@
           <t>3 - 2</t>
         </is>
       </c>
-      <c r="J103" s="108" t="n">
+      <c r="J103" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K103" s="2" t="n"/>
@@ -6297,7 +6312,7 @@
           <t>5 - 2</t>
         </is>
       </c>
-      <c r="J104" s="110" t="n">
+      <c r="J104" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K104" s="2" t="n"/>
@@ -6349,7 +6364,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J105" s="110" t="n">
+      <c r="J105" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K105" s="2" t="n"/>
@@ -6401,7 +6416,7 @@
           <t>3 - 1</t>
         </is>
       </c>
-      <c r="J106" s="110" t="n">
+      <c r="J106" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K106" s="2" t="n"/>
@@ -6453,7 +6468,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J107" s="110" t="n">
+      <c r="J107" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K107" s="2" t="n"/>
@@ -6505,7 +6520,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J108" s="110" t="n">
+      <c r="J108" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K108" s="2" t="n"/>
@@ -6557,7 +6572,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J109" s="108" t="n">
+      <c r="J109" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K109" s="2" t="n"/>
@@ -6609,7 +6624,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J110" s="110" t="n">
+      <c r="J110" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K110" s="2" t="n"/>
@@ -6661,7 +6676,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J111" s="110" t="n">
+      <c r="J111" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K111" s="2" t="n"/>
@@ -6713,7 +6728,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J112" s="110" t="n">
+      <c r="J112" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K112" s="2" t="n"/>
@@ -6765,7 +6780,7 @@
           <t>0 - 4</t>
         </is>
       </c>
-      <c r="J113" s="110" t="n">
+      <c r="J113" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K113" s="2" t="n"/>
@@ -6817,7 +6832,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J114" s="110" t="n">
+      <c r="J114" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K114" s="2" t="n"/>
@@ -6869,7 +6884,7 @@
           <t>4 - 3</t>
         </is>
       </c>
-      <c r="J115" s="110" t="n">
+      <c r="J115" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K115" s="2" t="n"/>
@@ -6921,7 +6936,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J116" s="110" t="n">
+      <c r="J116" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K116" s="2" t="n"/>
@@ -6973,7 +6988,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J117" s="110" t="n">
+      <c r="J117" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K117" s="2" t="n"/>
@@ -7025,7 +7040,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J118" s="110" t="n">
+      <c r="J118" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K118" s="2" t="n"/>
@@ -7077,7 +7092,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J119" s="108" t="n">
+      <c r="J119" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K119" s="2" t="n"/>
@@ -7129,7 +7144,7 @@
           <t>0 - 4</t>
         </is>
       </c>
-      <c r="J120" s="110" t="n">
+      <c r="J120" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K120" s="2" t="n"/>
@@ -7181,7 +7196,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J121" s="110" t="n">
+      <c r="J121" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K121" s="2" t="n"/>
@@ -7233,7 +7248,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J122" s="108" t="n">
+      <c r="J122" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K122" s="2" t="n"/>
@@ -7285,7 +7300,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J123" s="110" t="n">
+      <c r="J123" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K123" s="2" t="n"/>
@@ -7337,7 +7352,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J124" s="110" t="n">
+      <c r="J124" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K124" s="2" t="n"/>
@@ -7389,7 +7404,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J125" s="110" t="n">
+      <c r="J125" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K125" s="2" t="n"/>
@@ -7441,7 +7456,7 @@
           <t>0 - 0</t>
         </is>
       </c>
-      <c r="J126" s="108" t="n">
+      <c r="J126" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K126" s="2" t="n"/>
@@ -7493,7 +7508,7 @@
           <t>1 - 3</t>
         </is>
       </c>
-      <c r="J127" s="110" t="n">
+      <c r="J127" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K127" s="2" t="n"/>
@@ -7545,7 +7560,7 @@
           <t>1 - 4</t>
         </is>
       </c>
-      <c r="J128" s="110" t="n">
+      <c r="J128" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K128" s="2" t="n"/>
@@ -7597,7 +7612,7 @@
           <t>4 - 0</t>
         </is>
       </c>
-      <c r="J129" s="110" t="n">
+      <c r="J129" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K129" s="2" t="n"/>
@@ -7649,7 +7664,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J130" s="108" t="n">
+      <c r="J130" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K130" s="2" t="n"/>
@@ -7701,7 +7716,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J131" s="110" t="n">
+      <c r="J131" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K131" s="2" t="n"/>
@@ -7753,7 +7768,7 @@
           <t>0 - 4</t>
         </is>
       </c>
-      <c r="J132" s="110" t="n">
+      <c r="J132" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K132" s="2" t="n"/>
@@ -7805,7 +7820,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J133" s="110" t="n">
+      <c r="J133" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K133" s="2" t="n"/>
@@ -7857,7 +7872,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J134" s="110" t="n">
+      <c r="J134" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K134" s="2" t="n"/>
@@ -7909,7 +7924,7 @@
           <t>4 - 2</t>
         </is>
       </c>
-      <c r="J135" s="110" t="n">
+      <c r="J135" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K135" s="2" t="n"/>
@@ -7961,7 +7976,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J136" s="110" t="n">
+      <c r="J136" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K136" s="2" t="n"/>
@@ -8013,7 +8028,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J137" s="110" t="n">
+      <c r="J137" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K137" s="2" t="n"/>
@@ -8065,7 +8080,7 @@
           <t>5 - 0</t>
         </is>
       </c>
-      <c r="J138" s="110" t="n">
+      <c r="J138" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K138" s="2" t="n"/>
@@ -8117,7 +8132,7 @@
           <t>2 - 3</t>
         </is>
       </c>
-      <c r="J139" s="110" t="n">
+      <c r="J139" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K139" s="2" t="n"/>
@@ -8169,7 +8184,7 @@
           <t>0 - 2</t>
         </is>
       </c>
-      <c r="J140" s="110" t="n">
+      <c r="J140" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K140" s="2" t="n"/>
@@ -8221,7 +8236,7 @@
           <t>0 - 3</t>
         </is>
       </c>
-      <c r="J141" s="110" t="n">
+      <c r="J141" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K141" s="2" t="n"/>
@@ -8273,7 +8288,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J142" s="110" t="n">
+      <c r="J142" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K142" s="2" t="n"/>
@@ -8325,7 +8340,7 @@
           <t>1 - 2</t>
         </is>
       </c>
-      <c r="J143" s="108" t="n">
+      <c r="J143" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K143" s="2" t="n"/>
@@ -8377,7 +8392,7 @@
           <t>4 - 0</t>
         </is>
       </c>
-      <c r="J144" s="110" t="n">
+      <c r="J144" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K144" s="2" t="n"/>
@@ -8429,7 +8444,7 @@
           <t>2 - 2</t>
         </is>
       </c>
-      <c r="J145" s="108" t="n">
+      <c r="J145" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K145" s="2" t="n"/>
@@ -8481,7 +8496,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J146" s="110" t="n">
+      <c r="J146" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K146" s="2" t="n"/>
@@ -8533,7 +8548,7 @@
           <t>0 - 1</t>
         </is>
       </c>
-      <c r="J147" s="110" t="n">
+      <c r="J147" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K147" s="2" t="n"/>
@@ -8585,7 +8600,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J148" s="110" t="n">
+      <c r="J148" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K148" s="2" t="n"/>
@@ -8637,7 +8652,7 @@
           <t>1 - 0</t>
         </is>
       </c>
-      <c r="J149" s="108" t="n">
+      <c r="J149" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K149" s="2" t="n"/>
@@ -8689,7 +8704,7 @@
           <t>2 - 0</t>
         </is>
       </c>
-      <c r="J150" s="110" t="n">
+      <c r="J150" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K150" s="2" t="n"/>
@@ -8741,7 +8756,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J151" s="110" t="n">
+      <c r="J151" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K151" s="2" t="n"/>
@@ -8793,7 +8808,7 @@
           <t>1 - 4</t>
         </is>
       </c>
-      <c r="J152" s="110" t="n">
+      <c r="J152" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K152" s="2" t="n"/>
@@ -8845,7 +8860,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J153" s="108" t="n">
+      <c r="J153" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K153" s="2" t="n"/>
@@ -8897,7 +8912,7 @@
           <t>4 - 1</t>
         </is>
       </c>
-      <c r="J154" s="108" t="n">
+      <c r="J154" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K154" s="2" t="n"/>
@@ -8949,7 +8964,7 @@
           <t>3 - 0</t>
         </is>
       </c>
-      <c r="J155" s="108" t="n">
+      <c r="J155" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K155" s="2" t="n"/>
@@ -9001,7 +9016,7 @@
           <t>3 - 4</t>
         </is>
       </c>
-      <c r="J156" s="108" t="n">
+      <c r="J156" s="114" t="n">
         <v>0</v>
       </c>
       <c r="K156" s="2" t="n"/>
@@ -9053,7 +9068,7 @@
           <t>1 - 1</t>
         </is>
       </c>
-      <c r="J157" s="110" t="n">
+      <c r="J157" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K157" s="2" t="n"/>
@@ -9105,7 +9120,7 @@
           <t>5 - 2</t>
         </is>
       </c>
-      <c r="J158" s="110" t="n">
+      <c r="J158" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K158" s="2" t="n"/>
@@ -9157,7 +9172,7 @@
           <t>2 - 1</t>
         </is>
       </c>
-      <c r="J159" s="110" t="n">
+      <c r="J159" s="115" t="n">
         <v>1</v>
       </c>
       <c r="K159" s="2" t="n"/>
@@ -9170,6 +9185,266 @@
       <c r="R159" s="2" t="n"/>
       <c r="S159" s="2" t="n"/>
       <c r="T159" s="2" t="n"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="2" t="inlineStr">
+        <is>
+          <t>24.09.2025</t>
+        </is>
+      </c>
+      <c r="B160" s="2" t="inlineStr">
+        <is>
+          <t>Atletico Madrid</t>
+        </is>
+      </c>
+      <c r="C160" s="2" t="inlineStr">
+        <is>
+          <t>Rayo Vallecano</t>
+        </is>
+      </c>
+      <c r="D160" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E160" s="2" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="F160" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G160" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="H160" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="I160" s="2" t="inlineStr">
+        <is>
+          <t>3 - 2</t>
+        </is>
+      </c>
+      <c r="J160" s="115" t="n">
+        <v>1</v>
+      </c>
+      <c r="K160" s="2" t="n"/>
+      <c r="L160" s="2" t="n"/>
+      <c r="M160" s="2" t="n"/>
+      <c r="N160" s="2" t="n"/>
+      <c r="O160" s="2" t="n"/>
+      <c r="P160" s="2" t="n"/>
+      <c r="Q160" s="2" t="n"/>
+      <c r="R160" s="2" t="n"/>
+      <c r="S160" s="2" t="n"/>
+      <c r="T160" s="2" t="n"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="inlineStr">
+        <is>
+          <t>27.09.2025</t>
+        </is>
+      </c>
+      <c r="B161" s="2" t="inlineStr">
+        <is>
+          <t>Crystal Palace</t>
+        </is>
+      </c>
+      <c r="C161" s="2" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="D161" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E161" s="2" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="F161" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G161" s="2" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="H161" s="2" t="n">
+        <v>8.799999999999997</v>
+      </c>
+      <c r="I161" s="2" t="inlineStr">
+        <is>
+          <t>2 - 1</t>
+        </is>
+      </c>
+      <c r="J161" s="114" t="n">
+        <v>0</v>
+      </c>
+      <c r="K161" s="2" t="n"/>
+      <c r="L161" s="2" t="n"/>
+      <c r="M161" s="2" t="n"/>
+      <c r="N161" s="2" t="n"/>
+      <c r="O161" s="2" t="n"/>
+      <c r="P161" s="2" t="n"/>
+      <c r="Q161" s="2" t="n"/>
+      <c r="R161" s="2" t="n"/>
+      <c r="S161" s="2" t="n"/>
+      <c r="T161" s="2" t="n"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="inlineStr">
+        <is>
+          <t>27.09.2025</t>
+        </is>
+      </c>
+      <c r="B162" s="2" t="inlineStr">
+        <is>
+          <t>Lorient</t>
+        </is>
+      </c>
+      <c r="C162" s="2" t="inlineStr">
+        <is>
+          <t>Monaco</t>
+        </is>
+      </c>
+      <c r="D162" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E162" s="2" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="F162" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G162" s="2" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="H162" s="2" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="I162" s="2" t="inlineStr">
+        <is>
+          <t>3 - 1</t>
+        </is>
+      </c>
+      <c r="J162" s="114" t="n">
+        <v>0</v>
+      </c>
+      <c r="K162" s="2" t="n"/>
+      <c r="L162" s="2" t="n"/>
+      <c r="M162" s="2" t="n"/>
+      <c r="N162" s="2" t="n"/>
+      <c r="O162" s="2" t="n"/>
+      <c r="P162" s="2" t="n"/>
+      <c r="Q162" s="2" t="n"/>
+      <c r="R162" s="2" t="n"/>
+      <c r="S162" s="2" t="n"/>
+      <c r="T162" s="2" t="n"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="inlineStr">
+        <is>
+          <t>27.09.2025</t>
+        </is>
+      </c>
+      <c r="B163" s="2" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="C163" s="2" t="inlineStr">
+        <is>
+          <t>Inter Milan</t>
+        </is>
+      </c>
+      <c r="D163" s="2" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="E163" s="2" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="F163" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G163" s="2" t="n">
+        <v>56.99999999999999</v>
+      </c>
+      <c r="H163" s="2" t="n">
+        <v>6.999999999999993</v>
+      </c>
+      <c r="I163" s="2" t="inlineStr">
+        <is>
+          <t>0 - 2</t>
+        </is>
+      </c>
+      <c r="J163" s="115" t="n">
+        <v>1</v>
+      </c>
+      <c r="K163" s="2" t="n"/>
+      <c r="L163" s="2" t="n"/>
+      <c r="M163" s="2" t="n"/>
+      <c r="N163" s="2" t="n"/>
+      <c r="O163" s="2" t="n"/>
+      <c r="P163" s="2" t="n"/>
+      <c r="Q163" s="2" t="n"/>
+      <c r="R163" s="2" t="n"/>
+      <c r="S163" s="2" t="n"/>
+      <c r="T163" s="2" t="n"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="inlineStr">
+        <is>
+          <t>27.09.2025</t>
+        </is>
+      </c>
+      <c r="B164" s="2" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="C164" s="2" t="inlineStr">
+        <is>
+          <t>Auxerre</t>
+        </is>
+      </c>
+      <c r="D164" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E164" s="2" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="F164" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G164" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="H164" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="I164" s="2" t="inlineStr">
+        <is>
+          <t>2 - 0</t>
+        </is>
+      </c>
+      <c r="J164" s="115" t="n">
+        <v>1</v>
+      </c>
+      <c r="K164" s="2" t="n"/>
+      <c r="L164" s="2" t="n"/>
+      <c r="M164" s="2" t="n"/>
+      <c r="N164" s="2" t="n"/>
+      <c r="O164" s="2" t="n"/>
+      <c r="P164" s="2" t="n"/>
+      <c r="Q164" s="2" t="n"/>
+      <c r="R164" s="2" t="n"/>
+      <c r="S164" s="2" t="n"/>
+      <c r="T164" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9261,14 +9536,14 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>7</v>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>70.0%</t>
+          <t>63.64%</t>
         </is>
       </c>
     </row>
@@ -9315,14 +9590,14 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>54.55%</t>
+          <t>58.33%</t>
         </is>
       </c>
     </row>
@@ -9513,14 +9788,14 @@
         </is>
       </c>
       <c r="B18" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>11</v>
-      </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>91.67%</t>
+          <t>92.31%</t>
         </is>
       </c>
     </row>
@@ -9657,14 +9932,14 @@
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>75.0%</t>
+          <t>60.0%</t>
         </is>
       </c>
     </row>
@@ -9693,14 +9968,14 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>84.62%</t>
+          <t>85.71%</t>
         </is>
       </c>
     </row>

</xml_diff>